<commit_message>
closer population, better births and fixed 0-14 deaths
</commit_message>
<xml_diff>
--- a/parameters/DataWorkbookRubella.xlsx
+++ b/parameters/DataWorkbookRubella.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taahir/Downloads/RubellaNew/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taahir/Downloads/RubellaNew/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62143C7E-05F1-254C-B492-B29D98D150BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976F5D7C-BCBC-B34C-866D-DE8A4F27CF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{F270E22A-AF68-0948-A29A-BD37CB605717}"/>
   </bookViews>
@@ -2494,7 +2494,7 @@
   <dimension ref="A1:N144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="T85" sqref="T85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2559,7 +2559,7 @@
         <v>61140.011249999996</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <f>(K2/100)*G2</f>
@@ -2589,7 +2589,7 @@
       </c>
       <c r="M2" s="6">
         <f>SUM(C2:E2)-G2</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -2607,7 +2607,7 @@
         <v>61140.011249999996</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <f>(K3/100)*G3</f>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="M3" s="6">
         <f t="shared" ref="M3:M66" si="2">SUM(C3:E3)-G3</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -2655,10 +2655,10 @@
         <v>61140.011249999996</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E3:E66" si="3">(K4/100)*G4</f>
+        <f t="shared" ref="E4:E66" si="3">(K4/100)*G4</f>
         <v>18781.572083333333</v>
       </c>
       <c r="F4">
@@ -2685,7 +2685,7 @@
       </c>
       <c r="M4" s="6">
         <f>SUM(C4:E4)-G4</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -2703,7 +2703,7 @@
         <v>61140.011249999996</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <f t="shared" si="3"/>
@@ -2733,7 +2733,7 @@
       </c>
       <c r="M5" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -2751,7 +2751,7 @@
         <v>61140.011249999996</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <f t="shared" si="3"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="M6" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -2799,7 +2799,7 @@
         <v>61140.011249999996</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <f t="shared" si="3"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="M7" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -2847,7 +2847,7 @@
         <v>61140.011249999996</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <f t="shared" si="3"/>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="M8" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -2895,7 +2895,7 @@
         <v>61140.011249999996</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <f t="shared" si="3"/>
@@ -2925,7 +2925,7 @@
       </c>
       <c r="M9" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -2943,7 +2943,7 @@
         <v>61140.011249999996</v>
       </c>
       <c r="D10">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <f t="shared" si="3"/>
@@ -2973,7 +2973,7 @@
       </c>
       <c r="M10" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -2991,7 +2991,7 @@
         <v>61140.011249999996</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <f t="shared" si="3"/>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="M11" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -3039,7 +3039,7 @@
         <v>61140.011249999996</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E12">
         <f t="shared" si="3"/>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="M12" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -3087,7 +3087,7 @@
         <v>61140.011249999996</v>
       </c>
       <c r="D13">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E13">
         <f t="shared" si="3"/>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="M13" s="6">
         <f>SUM(C13:E13)-G13</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -3135,7 +3135,7 @@
         <v>58595.876250000001</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E14">
         <f t="shared" si="3"/>
@@ -3165,7 +3165,7 @@
       </c>
       <c r="M14" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -3183,7 +3183,7 @@
         <v>58595.876250000001</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E15">
         <f t="shared" si="3"/>
@@ -3213,7 +3213,7 @@
       </c>
       <c r="M15" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -3231,7 +3231,7 @@
         <v>58595.876250000001</v>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E16">
         <f t="shared" si="3"/>
@@ -3261,7 +3261,7 @@
       </c>
       <c r="M16" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N16">
         <v>1</v>
@@ -3279,7 +3279,7 @@
         <v>58595.876250000001</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <f t="shared" si="3"/>
@@ -3309,7 +3309,7 @@
       </c>
       <c r="M17" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N17">
         <v>1</v>
@@ -3327,7 +3327,7 @@
         <v>58595.876250000001</v>
       </c>
       <c r="D18">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E18">
         <f t="shared" si="3"/>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="M18" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N18">
         <v>1</v>
@@ -3375,7 +3375,7 @@
         <v>58595.876250000001</v>
       </c>
       <c r="D19">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E19">
         <f t="shared" si="3"/>
@@ -3405,7 +3405,7 @@
       </c>
       <c r="M19" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N19">
         <v>1</v>
@@ -3423,7 +3423,7 @@
         <v>58595.876250000001</v>
       </c>
       <c r="D20">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <f t="shared" si="3"/>
@@ -3453,7 +3453,7 @@
       </c>
       <c r="M20" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N20">
         <v>1</v>
@@ -3471,7 +3471,7 @@
         <v>58595.876250000001</v>
       </c>
       <c r="D21">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E21">
         <f t="shared" si="3"/>
@@ -3501,7 +3501,7 @@
       </c>
       <c r="M21" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N21">
         <v>1</v>
@@ -3519,7 +3519,7 @@
         <v>58595.876250000001</v>
       </c>
       <c r="D22">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E22">
         <f t="shared" si="3"/>
@@ -3549,7 +3549,7 @@
       </c>
       <c r="M22" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N22">
         <v>1</v>
@@ -3567,7 +3567,7 @@
         <v>58595.876250000001</v>
       </c>
       <c r="D23">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E23">
         <f t="shared" si="3"/>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="M23" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N23">
         <v>1</v>
@@ -3615,7 +3615,7 @@
         <v>58595.876250000001</v>
       </c>
       <c r="D24">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E24">
         <f t="shared" si="3"/>
@@ -3645,7 +3645,7 @@
       </c>
       <c r="M24" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N24">
         <v>1</v>
@@ -3663,7 +3663,7 @@
         <v>58595.876250000001</v>
       </c>
       <c r="D25">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E25">
         <f t="shared" si="3"/>
@@ -3693,7 +3693,7 @@
       </c>
       <c r="M25" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N25">
         <v>1</v>
@@ -3711,7 +3711,7 @@
         <v>59374.77375</v>
       </c>
       <c r="D26">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E26">
         <f t="shared" si="3"/>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="M26" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N26">
         <v>1</v>
@@ -3759,7 +3759,7 @@
         <v>59374.77375</v>
       </c>
       <c r="D27">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E27">
         <f t="shared" si="3"/>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="M27" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N27">
         <v>1</v>
@@ -3807,7 +3807,7 @@
         <v>59374.77375</v>
       </c>
       <c r="D28">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E28">
         <f t="shared" si="3"/>
@@ -3837,7 +3837,7 @@
       </c>
       <c r="M28" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N28">
         <v>1</v>
@@ -3855,7 +3855,7 @@
         <v>59374.77375</v>
       </c>
       <c r="D29">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E29">
         <f t="shared" si="3"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="M29" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N29">
         <v>1</v>
@@ -3903,7 +3903,7 @@
         <v>59374.77375</v>
       </c>
       <c r="D30">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E30">
         <f t="shared" si="3"/>
@@ -3933,7 +3933,7 @@
       </c>
       <c r="M30" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N30">
         <v>1</v>
@@ -3951,7 +3951,7 @@
         <v>59374.77375</v>
       </c>
       <c r="D31">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E31">
         <f t="shared" si="3"/>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="M31" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N31">
         <v>1</v>
@@ -3999,7 +3999,7 @@
         <v>59374.77375</v>
       </c>
       <c r="D32">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E32">
         <f t="shared" si="3"/>
@@ -4029,7 +4029,7 @@
       </c>
       <c r="M32" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N32">
         <v>1</v>
@@ -4047,7 +4047,7 @@
         <v>59374.77375</v>
       </c>
       <c r="D33">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E33">
         <f t="shared" si="3"/>
@@ -4077,7 +4077,7 @@
       </c>
       <c r="M33" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N33">
         <v>1</v>
@@ -4095,7 +4095,7 @@
         <v>59374.77375</v>
       </c>
       <c r="D34">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E34">
         <f t="shared" si="3"/>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="M34" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N34">
         <v>1</v>
@@ -4143,7 +4143,7 @@
         <v>59374.77375</v>
       </c>
       <c r="D35">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E35">
         <f t="shared" si="3"/>
@@ -4173,7 +4173,7 @@
       </c>
       <c r="M35" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N35">
         <v>1</v>
@@ -4191,7 +4191,7 @@
         <v>59374.77375</v>
       </c>
       <c r="D36">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E36">
         <f t="shared" si="3"/>
@@ -4221,7 +4221,7 @@
       </c>
       <c r="M36" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N36">
         <v>1</v>
@@ -4239,7 +4239,7 @@
         <v>59374.77375</v>
       </c>
       <c r="D37">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E37">
         <f t="shared" si="3"/>
@@ -4269,7 +4269,7 @@
       </c>
       <c r="M37" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N37">
         <v>1</v>
@@ -4287,7 +4287,7 @@
         <v>61600.86</v>
       </c>
       <c r="D38">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E38">
         <f t="shared" si="3"/>
@@ -4317,7 +4317,7 @@
       </c>
       <c r="M38" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N38">
         <v>1</v>
@@ -4335,7 +4335,7 @@
         <v>61600.86</v>
       </c>
       <c r="D39">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E39">
         <f t="shared" si="3"/>
@@ -4365,7 +4365,7 @@
       </c>
       <c r="M39" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N39">
         <v>1</v>
@@ -4383,7 +4383,7 @@
         <v>61600.86</v>
       </c>
       <c r="D40">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E40">
         <f t="shared" si="3"/>
@@ -4413,7 +4413,7 @@
       </c>
       <c r="M40" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N40">
         <v>1</v>
@@ -4431,7 +4431,7 @@
         <v>61600.86</v>
       </c>
       <c r="D41">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E41">
         <f t="shared" si="3"/>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="M41" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N41">
         <v>1</v>
@@ -4479,7 +4479,7 @@
         <v>61600.86</v>
       </c>
       <c r="D42">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E42">
         <f t="shared" si="3"/>
@@ -4509,7 +4509,7 @@
       </c>
       <c r="M42" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N42">
         <v>1</v>
@@ -4527,7 +4527,7 @@
         <v>61600.86</v>
       </c>
       <c r="D43">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E43">
         <f t="shared" si="3"/>
@@ -4557,7 +4557,7 @@
       </c>
       <c r="M43" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N43">
         <v>1</v>
@@ -4575,7 +4575,7 @@
         <v>61600.86</v>
       </c>
       <c r="D44">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E44">
         <f t="shared" si="3"/>
@@ -4605,7 +4605,7 @@
       </c>
       <c r="M44" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N44">
         <v>1</v>
@@ -4623,7 +4623,7 @@
         <v>61600.86</v>
       </c>
       <c r="D45">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E45">
         <f t="shared" si="3"/>
@@ -4633,7 +4633,7 @@
         <v>0</v>
       </c>
       <c r="G45" s="6">
-        <f t="shared" si="1"/>
+        <f>(I45+J45)/12</f>
         <v>80524</v>
       </c>
       <c r="H45" s="1" t="s">
@@ -4653,7 +4653,7 @@
       </c>
       <c r="M45" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N45">
         <v>1</v>
@@ -4671,7 +4671,7 @@
         <v>61600.86</v>
       </c>
       <c r="D46">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E46">
         <f t="shared" si="3"/>
@@ -4701,7 +4701,7 @@
       </c>
       <c r="M46" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N46">
         <v>1</v>
@@ -4719,7 +4719,7 @@
         <v>61600.86</v>
       </c>
       <c r="D47">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E47">
         <f t="shared" si="3"/>
@@ -4749,7 +4749,7 @@
       </c>
       <c r="M47" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N47">
         <v>1</v>
@@ -4767,7 +4767,7 @@
         <v>61600.86</v>
       </c>
       <c r="D48">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E48">
         <f t="shared" si="3"/>
@@ -4797,7 +4797,7 @@
       </c>
       <c r="M48" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N48">
         <v>1</v>
@@ -4815,7 +4815,7 @@
         <v>61600.86</v>
       </c>
       <c r="D49">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E49">
         <f t="shared" si="3"/>
@@ -4845,7 +4845,7 @@
       </c>
       <c r="M49" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N49">
         <v>1</v>
@@ -4863,7 +4863,7 @@
         <v>724268.34</v>
       </c>
       <c r="D50">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E50">
         <f t="shared" si="3"/>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="M50" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N50">
         <v>1</v>
@@ -4911,7 +4911,7 @@
         <v>382644.50400000002</v>
       </c>
       <c r="D51">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E51">
         <f t="shared" si="3"/>
@@ -4941,7 +4941,7 @@
       </c>
       <c r="M51" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N51">
         <v>1</v>
@@ -4959,7 +4959,7 @@
         <v>383901.96</v>
       </c>
       <c r="D52">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E52">
         <f t="shared" si="3"/>
@@ -4989,7 +4989,7 @@
       </c>
       <c r="M52" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N52">
         <v>1</v>
@@ -5007,7 +5007,7 @@
         <v>386153.96400000004</v>
       </c>
       <c r="D53">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E53">
         <f t="shared" si="3"/>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="M53" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N53">
         <v>1</v>
@@ -5055,7 +5055,7 @@
         <v>388522.14600000001</v>
       </c>
       <c r="D54">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E54">
         <f t="shared" si="3"/>
@@ -5085,7 +5085,7 @@
       </c>
       <c r="M54" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N54">
         <v>1</v>
@@ -5103,7 +5103,7 @@
         <v>391383.984</v>
       </c>
       <c r="D55">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E55">
         <f t="shared" si="3"/>
@@ -5133,7 +5133,7 @@
       </c>
       <c r="M55" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N55">
         <v>1</v>
@@ -5151,7 +5151,7 @@
         <v>170117.12800000003</v>
       </c>
       <c r="D56">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E56">
         <f t="shared" si="3"/>
@@ -5181,7 +5181,7 @@
       </c>
       <c r="M56" s="6">
         <f t="shared" si="2"/>
-        <v>10.000000000116415</v>
+        <v>3.0000000001164153</v>
       </c>
       <c r="N56">
         <v>1</v>
@@ -5199,7 +5199,7 @@
         <v>171482.27100000001</v>
       </c>
       <c r="D57">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E57">
         <f t="shared" si="3"/>
@@ -5229,7 +5229,7 @@
       </c>
       <c r="M57" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N57">
         <v>1</v>
@@ -5247,7 +5247,7 @@
         <v>173080.27200000003</v>
       </c>
       <c r="D58">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E58">
         <f t="shared" si="3"/>
@@ -5277,7 +5277,7 @@
       </c>
       <c r="M58" s="6">
         <f t="shared" si="2"/>
-        <v>10.000000000116415</v>
+        <v>3.0000000001164153</v>
       </c>
       <c r="N58">
         <v>1</v>
@@ -5295,7 +5295,7 @@
         <v>174552.67500000002</v>
       </c>
       <c r="D59">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E59">
         <f t="shared" si="3"/>
@@ -5325,7 +5325,7 @@
       </c>
       <c r="M59" s="6">
         <f t="shared" si="2"/>
-        <v>10.000000000116415</v>
+        <v>3.0000000001164153</v>
       </c>
       <c r="N59">
         <v>1</v>
@@ -5343,7 +5343,7 @@
         <v>175646.38100000002</v>
       </c>
       <c r="D60">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E60">
         <f t="shared" si="3"/>
@@ -5373,7 +5373,7 @@
       </c>
       <c r="M60" s="6">
         <f t="shared" si="2"/>
-        <v>10.000000000116415</v>
+        <v>3.0000000001164153</v>
       </c>
       <c r="N60">
         <v>1</v>
@@ -5391,7 +5391,7 @@
         <v>86199.95</v>
       </c>
       <c r="D61">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E61">
         <f t="shared" si="3"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="M61" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N61">
         <v>2</v>
@@ -5439,7 +5439,7 @@
         <v>85549.617999999988</v>
       </c>
       <c r="D62">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E62">
         <f t="shared" si="3"/>
@@ -5469,7 +5469,7 @@
       </c>
       <c r="M62" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N62">
         <v>2</v>
@@ -5487,7 +5487,7 @@
         <v>83921.207999999999</v>
       </c>
       <c r="D63">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E63">
         <f t="shared" si="3"/>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="M63" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N63">
         <v>2</v>
@@ -5535,7 +5535,7 @@
         <v>81463.757999999987</v>
       </c>
       <c r="D64">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E64">
         <f t="shared" si="3"/>
@@ -5565,7 +5565,7 @@
       </c>
       <c r="M64" s="6">
         <f t="shared" si="2"/>
-        <v>10.000000000116415</v>
+        <v>3.0000000001164153</v>
       </c>
       <c r="N64">
         <v>2</v>
@@ -5583,7 +5583,7 @@
         <v>78593.25</v>
       </c>
       <c r="D65">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E65">
         <f t="shared" si="3"/>
@@ -5613,7 +5613,7 @@
       </c>
       <c r="M65" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N65">
         <v>2</v>
@@ -5631,7 +5631,7 @@
         <v>65325.202000000012</v>
       </c>
       <c r="D66">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E66">
         <f t="shared" si="3"/>
@@ -5661,7 +5661,7 @@
       </c>
       <c r="M66" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N66">
         <v>3</v>
@@ -5679,7 +5679,7 @@
         <v>63496.44000000001</v>
       </c>
       <c r="D67">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E67">
         <f t="shared" ref="E67:E109" si="6">(K67/100)*G67</f>
@@ -5709,7 +5709,7 @@
       </c>
       <c r="M67" s="6">
         <f t="shared" ref="M67:M109" si="8">SUM(C67:E67)-G67</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N67">
         <v>3</v>
@@ -5727,7 +5727,7 @@
         <v>62418.556000000011</v>
       </c>
       <c r="D68">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E68">
         <f t="shared" si="6"/>
@@ -5757,7 +5757,7 @@
       </c>
       <c r="M68" s="6">
         <f t="shared" si="8"/>
-        <v>9.9999999998835847</v>
+        <v>2.9999999998835847</v>
       </c>
       <c r="N68">
         <v>3</v>
@@ -5775,7 +5775,7 @@
         <v>61885.534000000007</v>
       </c>
       <c r="D69">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E69">
         <f t="shared" si="6"/>
@@ -5805,7 +5805,7 @@
       </c>
       <c r="M69" s="6">
         <f t="shared" si="8"/>
-        <v>9.9999999998835847</v>
+        <v>2.9999999998835847</v>
       </c>
       <c r="N69">
         <v>3</v>
@@ -5823,7 +5823,7 @@
         <v>61515.386000000006</v>
       </c>
       <c r="D70">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E70">
         <f t="shared" si="6"/>
@@ -5853,7 +5853,7 @@
       </c>
       <c r="M70" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N70">
         <v>3</v>
@@ -5871,7 +5871,7 @@
         <v>58387.133999999998</v>
       </c>
       <c r="D71">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E71">
         <f t="shared" si="6"/>
@@ -5901,7 +5901,7 @@
       </c>
       <c r="M71" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N71">
         <v>4</v>
@@ -5919,7 +5919,7 @@
         <v>57328.95</v>
       </c>
       <c r="D72">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E72">
         <f t="shared" si="6"/>
@@ -5949,7 +5949,7 @@
       </c>
       <c r="M72" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N72">
         <v>4</v>
@@ -5967,7 +5967,7 @@
         <v>55701.842999999993</v>
       </c>
       <c r="D73">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E73">
         <f t="shared" si="6"/>
@@ -5997,7 +5997,7 @@
       </c>
       <c r="M73" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N73">
         <v>4</v>
@@ -6015,7 +6015,7 @@
         <v>53690.270999999993</v>
       </c>
       <c r="D74">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E74">
         <f t="shared" si="6"/>
@@ -6045,7 +6045,7 @@
       </c>
       <c r="M74" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N74">
         <v>4</v>
@@ -6063,7 +6063,7 @@
         <v>51559.986999999994</v>
       </c>
       <c r="D75">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E75">
         <f t="shared" si="6"/>
@@ -6093,7 +6093,7 @@
       </c>
       <c r="M75" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N75">
         <v>4</v>
@@ -6111,7 +6111,7 @@
         <v>53849.873</v>
       </c>
       <c r="D76">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E76">
         <f t="shared" si="6"/>
@@ -6141,7 +6141,7 @@
       </c>
       <c r="M76" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N76">
         <v>5</v>
@@ -6159,7 +6159,7 @@
         <v>52201.072</v>
       </c>
       <c r="D77">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E77">
         <f t="shared" si="6"/>
@@ -6189,7 +6189,7 @@
       </c>
       <c r="M77" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N77">
         <v>5</v>
@@ -6207,7 +6207,7 @@
         <v>51118.375</v>
       </c>
       <c r="D78">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E78">
         <f t="shared" si="6"/>
@@ -6237,7 +6237,7 @@
       </c>
       <c r="M78" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N78">
         <v>5</v>
@@ -6255,7 +6255,7 @@
         <v>50415.442000000003</v>
       </c>
       <c r="D79">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E79">
         <f t="shared" si="6"/>
@@ -6285,7 +6285,7 @@
       </c>
       <c r="M79" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N79">
         <v>5</v>
@@ -6303,7 +6303,7 @@
         <v>49818.923000000003</v>
       </c>
       <c r="D80">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E80">
         <f t="shared" si="6"/>
@@ -6333,7 +6333,7 @@
       </c>
       <c r="M80" s="6">
         <f t="shared" si="8"/>
-        <v>9.9999999998835847</v>
+        <v>2.9999999998835847</v>
       </c>
       <c r="N80">
         <v>5</v>
@@ -6351,7 +6351,7 @@
         <v>57362.85</v>
       </c>
       <c r="D81">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E81">
         <f t="shared" si="6"/>
@@ -6381,7 +6381,7 @@
       </c>
       <c r="M81" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N81">
         <v>6</v>
@@ -6399,7 +6399,7 @@
         <v>56287.89</v>
       </c>
       <c r="D82">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E82">
         <f t="shared" si="6"/>
@@ -6429,7 +6429,7 @@
       </c>
       <c r="M82" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N82">
         <v>6</v>
@@ -6447,7 +6447,7 @@
         <v>54860.49</v>
       </c>
       <c r="D83">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E83">
         <f t="shared" si="6"/>
@@ -6477,7 +6477,7 @@
       </c>
       <c r="M83" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N83">
         <v>6</v>
@@ -6495,7 +6495,7 @@
         <v>53154</v>
       </c>
       <c r="D84">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E84">
         <f t="shared" si="6"/>
@@ -6525,7 +6525,7 @@
       </c>
       <c r="M84" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N84">
         <v>6</v>
@@ -6543,7 +6543,7 @@
         <v>51376.409999999996</v>
       </c>
       <c r="D85">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E85">
         <f t="shared" si="6"/>
@@ -6573,7 +6573,7 @@
       </c>
       <c r="M85" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N85">
         <v>6</v>
@@ -6591,7 +6591,7 @@
         <v>52364.855000000003</v>
       </c>
       <c r="D86">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E86">
         <f t="shared" si="6"/>
@@ -6621,7 +6621,7 @@
       </c>
       <c r="M86" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N86">
         <v>7</v>
@@ -6639,7 +6639,7 @@
         <v>50386.004999999997</v>
       </c>
       <c r="D87">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E87">
         <f t="shared" si="6"/>
@@ -6669,7 +6669,7 @@
       </c>
       <c r="M87" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N87">
         <v>7</v>
@@ -6687,7 +6687,7 @@
         <v>48322.224999999999</v>
       </c>
       <c r="D88">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E88">
         <f t="shared" si="6"/>
@@ -6717,7 +6717,7 @@
       </c>
       <c r="M88" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N88">
         <v>7</v>
@@ -6735,7 +6735,7 @@
         <v>46212.18</v>
       </c>
       <c r="D89">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E89">
         <f t="shared" si="6"/>
@@ -6765,7 +6765,7 @@
       </c>
       <c r="M89" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N89">
         <v>7</v>
@@ -6783,7 +6783,7 @@
         <v>44076.01</v>
       </c>
       <c r="D90">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E90">
         <f t="shared" si="6"/>
@@ -6813,7 +6813,7 @@
       </c>
       <c r="M90" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N90">
         <v>7</v>
@@ -6831,7 +6831,7 @@
         <v>40642.932000000001</v>
       </c>
       <c r="D91">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E91">
         <f t="shared" si="6"/>
@@ -6861,7 +6861,7 @@
       </c>
       <c r="M91" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N91">
         <v>8</v>
@@ -6879,7 +6879,7 @@
         <v>38688.300000000003</v>
       </c>
       <c r="D92">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E92">
         <f t="shared" si="6"/>
@@ -6909,7 +6909,7 @@
       </c>
       <c r="M92" s="6">
         <f t="shared" si="8"/>
-        <v>9.9999999999417923</v>
+        <v>2.9999999999417923</v>
       </c>
       <c r="N92">
         <v>8</v>
@@ -6927,7 +6927,7 @@
         <v>36852.716</v>
       </c>
       <c r="D93">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E93">
         <f t="shared" si="6"/>
@@ -6957,7 +6957,7 @@
       </c>
       <c r="M93" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N93">
         <v>8</v>
@@ -6975,7 +6975,7 @@
         <v>35114.468000000001</v>
       </c>
       <c r="D94">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E94">
         <f t="shared" si="6"/>
@@ -7005,7 +7005,7 @@
       </c>
       <c r="M94" s="6">
         <f t="shared" si="8"/>
-        <v>9.9999999999417923</v>
+        <v>2.9999999999417923</v>
       </c>
       <c r="N94">
         <v>8</v>
@@ -7023,7 +7023,7 @@
         <v>33466.748</v>
       </c>
       <c r="D95">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E95">
         <f t="shared" si="6"/>
@@ -7053,7 +7053,7 @@
       </c>
       <c r="M95" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N95">
         <v>8</v>
@@ -7071,7 +7071,7 @@
         <v>37376.100000000006</v>
       </c>
       <c r="D96">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E96">
         <f t="shared" si="6"/>
@@ -7101,7 +7101,7 @@
       </c>
       <c r="M96" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N96">
         <v>9</v>
@@ -7119,7 +7119,7 @@
         <v>35406.504000000001</v>
       </c>
       <c r="D97">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E97">
         <f t="shared" si="6"/>
@@ -7149,7 +7149,7 @@
       </c>
       <c r="M97" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N97">
         <v>9</v>
@@ -7167,7 +7167,7 @@
         <v>33336.684000000001</v>
       </c>
       <c r="D98">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E98">
         <f t="shared" si="6"/>
@@ -7197,7 +7197,7 @@
       </c>
       <c r="M98" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N98">
         <v>9</v>
@@ -7215,7 +7215,7 @@
         <v>31241.592000000004</v>
       </c>
       <c r="D99">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E99">
         <f t="shared" si="6"/>
@@ -7245,7 +7245,7 @@
       </c>
       <c r="M99" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N99">
         <v>9</v>
@@ -7263,7 +7263,7 @@
         <v>29106.216000000004</v>
       </c>
       <c r="D100">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E100">
         <f t="shared" si="6"/>
@@ -7293,7 +7293,7 @@
       </c>
       <c r="M100" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N100">
         <v>9</v>
@@ -7311,7 +7311,7 @@
         <v>27151.416000000005</v>
       </c>
       <c r="D101">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E101">
         <f t="shared" si="6"/>
@@ -7341,7 +7341,7 @@
       </c>
       <c r="M101" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N101">
         <v>10</v>
@@ -7359,7 +7359,7 @@
         <v>25662.312000000002</v>
       </c>
       <c r="D102">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E102">
         <f t="shared" si="6"/>
@@ -7389,7 +7389,7 @@
       </c>
       <c r="M102" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N102">
         <v>10</v>
@@ -7407,7 +7407,7 @@
         <v>24787.404000000002</v>
       </c>
       <c r="D103">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E103">
         <f t="shared" si="6"/>
@@ -7437,7 +7437,7 @@
       </c>
       <c r="M103" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N103">
         <v>10</v>
@@ -7455,7 +7455,7 @@
         <v>24360.048000000003</v>
       </c>
       <c r="D104">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E104">
         <f t="shared" si="6"/>
@@ -7485,7 +7485,7 @@
       </c>
       <c r="M104" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N104">
         <v>10</v>
@@ -7503,7 +7503,7 @@
         <v>24155.712000000003</v>
       </c>
       <c r="D105">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E105">
         <f t="shared" si="6"/>
@@ -7533,7 +7533,7 @@
       </c>
       <c r="M105" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N105">
         <v>10</v>
@@ -7551,7 +7551,7 @@
         <v>193802.02560000005</v>
       </c>
       <c r="D106">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E106">
         <f t="shared" si="6"/>
@@ -7581,7 +7581,7 @@
       </c>
       <c r="M106" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N106">
         <v>1</v>
@@ -7599,7 +7599,7 @@
         <v>103144.79520000001</v>
       </c>
       <c r="D107">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E107">
         <f t="shared" si="6"/>
@@ -7629,7 +7629,7 @@
       </c>
       <c r="M107" s="6">
         <f t="shared" si="8"/>
-        <v>10.000000000116415</v>
+        <v>3.0000000001164153</v>
       </c>
       <c r="N107">
         <v>11</v>
@@ -7647,7 +7647,7 @@
         <v>38505.881520000003</v>
       </c>
       <c r="D108">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E108">
         <f t="shared" si="6"/>
@@ -7677,7 +7677,7 @@
       </c>
       <c r="M108" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N108">
         <v>11</v>
@@ -7695,7 +7695,7 @@
         <v>2482.8768</v>
       </c>
       <c r="D109">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E109">
         <f t="shared" si="6"/>
@@ -7725,7 +7725,7 @@
       </c>
       <c r="M109" s="6">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N109">
         <v>11</v>

</xml_diff>

<commit_message>
ptrans and longer run time
</commit_message>
<xml_diff>
--- a/parameters/DataWorkbookRubella.xlsx
+++ b/parameters/DataWorkbookRubella.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taahir/Downloads/RubellaNew/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECA4213-B0C8-C040-B8AC-100F4153A6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4673B739-9ACD-E145-8723-5727B388EDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="5" xr2:uid="{F270E22A-AF68-0948-A29A-BD37CB605717}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="6" xr2:uid="{F270E22A-AF68-0948-A29A-BD37CB605717}"/>
   </bookViews>
   <sheets>
     <sheet name="coverage_table " sheetId="1" r:id="rId1"/>
@@ -598,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -608,6 +608,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2530,7 +2531,7 @@
   <dimension ref="A1:N144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7905,7 +7906,7 @@
   <dimension ref="A1:O67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:H64"/>
+      <selection activeCell="F2" sqref="F2:F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7969,21 +7970,20 @@
       </c>
       <c r="D2">
         <f>(M2/100)*H2</f>
-        <v>366840.0675</v>
+        <v>394858.95750000002</v>
       </c>
       <c r="E2">
         <v>3</v>
       </c>
       <c r="F2">
         <f>(L2/100)*H2</f>
-        <v>112689.4325</v>
+        <v>121296.5425</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2" s="6">
-        <f>(J2+K2)/2</f>
-        <v>479529.5</v>
+      <c r="H2" s="9">
+        <v>516155.5</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="7">
@@ -8018,21 +8018,20 @@
       </c>
       <c r="D3">
         <f>(M3/100)*H3</f>
-        <v>366840.0675</v>
+        <v>383511.33</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3">
         <f>(L3/100)*H3</f>
-        <v>112689.4325</v>
+        <v>117810.67</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3" s="6">
-        <f>(J3+K3)/2</f>
-        <v>479529.5</v>
+      <c r="H3" s="9">
+        <v>501322</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="7">
@@ -8067,21 +8066,20 @@
       </c>
       <c r="D4">
         <f t="shared" ref="D4" si="0">(M4/100)*H4</f>
-        <v>703150.51500000001</v>
+        <v>767022.66</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4">
         <f t="shared" ref="F4:F64" si="1">(L4/100)*H4</f>
-        <v>216000.48499999999</v>
+        <v>235621.34</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4" s="6">
-        <f>(J4+K4)</f>
-        <v>919151</v>
+      <c r="H4" s="7">
+        <v>1002644</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="7">
@@ -8116,21 +8114,20 @@
       </c>
       <c r="D5">
         <f>(M5/100)*H5</f>
-        <v>712497.28500000003</v>
+        <v>745344.09</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>218871.715</v>
+        <v>228961.90999999997</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" s="6">
-        <f>(J5+K5)</f>
-        <v>931369</v>
+      <c r="H5" s="7">
+        <v>974306</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>35</v>
@@ -8167,21 +8164,20 @@
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D62" si="3">(M6/100)*H6</f>
-        <v>739210.32000000007</v>
+        <v>720550.44000000006</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>227077.68</v>
+        <v>221345.56</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6" s="6">
-        <f>(J6+K6)</f>
-        <v>966288</v>
+      <c r="H6" s="7">
+        <v>941896</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>47</v>
@@ -8218,21 +8214,20 @@
       </c>
       <c r="D7">
         <f t="shared" si="3"/>
-        <v>724268.34</v>
+        <v>692695.26</v>
       </c>
       <c r="E7">
         <v>3</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>222487.65999999997</v>
+        <v>212788.74</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7" s="6">
-        <f t="shared" ref="H7:H64" si="4">J7+K7</f>
-        <v>946756</v>
+      <c r="H7" s="7">
+        <v>905484</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>59</v>
@@ -8269,21 +8264,20 @@
       </c>
       <c r="D8">
         <f t="shared" si="3"/>
-        <v>382644.50400000002</v>
+        <v>350178.984</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>569207.49599999993</v>
+        <v>520913.016</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8" s="6">
-        <f t="shared" si="4"/>
-        <v>951852</v>
+      <c r="H8" s="7">
+        <v>871092</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>60</v>
@@ -8320,21 +8314,20 @@
       </c>
       <c r="D9">
         <f t="shared" si="3"/>
-        <v>383901.96</v>
+        <v>338841.37800000003</v>
       </c>
       <c r="E9">
         <v>3</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>571078.03999999992</v>
+        <v>504047.62199999997</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9" s="6">
-        <f t="shared" si="4"/>
-        <v>954980</v>
+      <c r="H9" s="7">
+        <v>842889</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>61</v>
@@ -8371,21 +8364,20 @@
       </c>
       <c r="D10">
         <f t="shared" si="3"/>
-        <v>386153.96400000004</v>
+        <v>331579.24800000002</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>574428.03599999996</v>
+        <v>493244.75199999998</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10" s="6">
-        <f t="shared" si="4"/>
-        <v>960582</v>
+      <c r="H10" s="7">
+        <v>824824</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>62</v>
@@ -8422,21 +8414,20 @@
       </c>
       <c r="D11">
         <f t="shared" si="3"/>
-        <v>388522.14600000001</v>
+        <v>327330.51</v>
       </c>
       <c r="E11">
         <v>3</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>577950.85399999993</v>
+        <v>486924.49</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11" s="6">
-        <f t="shared" si="4"/>
-        <v>966473</v>
+      <c r="H11" s="7">
+        <v>814255</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>63</v>
@@ -8473,21 +8464,20 @@
       </c>
       <c r="D12">
         <f t="shared" si="3"/>
-        <v>391383.984</v>
+        <v>324290.98800000001</v>
       </c>
       <c r="E12">
         <v>3</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>582208.01599999995</v>
+        <v>482403.01199999999</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="H12" s="6">
-        <f t="shared" si="4"/>
-        <v>973592</v>
+      <c r="H12" s="7">
+        <v>806694</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>64</v>
@@ -8524,21 +8514,20 @@
       </c>
       <c r="D13">
         <f t="shared" si="3"/>
-        <v>170117.12800000003</v>
+        <v>137730.49000000002</v>
       </c>
       <c r="E13">
         <v>3</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>813218.87200000009</v>
+        <v>658399.51</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13" s="6">
-        <f t="shared" si="4"/>
-        <v>983336</v>
+      <c r="H13" s="7">
+        <v>796130</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>65</v>
@@ -8557,7 +8546,7 @@
       </c>
       <c r="N13" s="6">
         <f t="shared" si="2"/>
-        <v>3.0000000001164153</v>
+        <v>3</v>
       </c>
       <c r="O13">
         <v>1</v>
@@ -8575,21 +8564,20 @@
       </c>
       <c r="D14">
         <f t="shared" si="3"/>
-        <v>171482.27100000001</v>
+        <v>134983.42300000001</v>
       </c>
       <c r="E14">
         <v>3</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>819744.72900000005</v>
+        <v>645267.57700000005</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="H14" s="6">
-        <f t="shared" si="4"/>
-        <v>991227</v>
+      <c r="H14" s="7">
+        <v>780251</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>66</v>
@@ -8626,21 +8614,20 @@
       </c>
       <c r="D15">
         <f t="shared" si="3"/>
-        <v>173080.27200000003</v>
+        <v>130949.92800000001</v>
       </c>
       <c r="E15">
         <v>3</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>827383.72800000012</v>
+        <v>625986.07200000004</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
-      <c r="H15" s="6">
-        <f t="shared" si="4"/>
-        <v>1000464</v>
+      <c r="H15" s="7">
+        <v>756936</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>67</v>
@@ -8659,7 +8646,7 @@
       </c>
       <c r="N15" s="6">
         <f t="shared" si="2"/>
-        <v>3.0000000001164153</v>
+        <v>3</v>
       </c>
       <c r="O15">
         <v>1</v>
@@ -8677,21 +8664,20 @@
       </c>
       <c r="D16">
         <f t="shared" si="3"/>
-        <v>174552.67500000002</v>
+        <v>126140.18200000002</v>
       </c>
       <c r="E16">
         <v>3</v>
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>834422.32500000007</v>
+        <v>602993.81800000009</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
-      <c r="H16" s="6">
-        <f t="shared" si="4"/>
-        <v>1008975</v>
+      <c r="H16" s="7">
+        <v>729134</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>68</v>
@@ -8728,21 +8714,20 @@
       </c>
       <c r="D17">
         <f t="shared" si="3"/>
-        <v>175646.38100000002</v>
+        <v>121213.31500000002</v>
       </c>
       <c r="E17">
         <v>3</v>
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>839650.61900000006</v>
+        <v>579441.68500000006</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
-      <c r="H17" s="6">
-        <f t="shared" si="4"/>
-        <v>1015297</v>
+      <c r="H17" s="7">
+        <v>700655</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>69</v>
@@ -8779,21 +8764,20 @@
       </c>
       <c r="D18">
         <f t="shared" si="3"/>
-        <v>86199.95</v>
+        <v>58170.141999999993</v>
       </c>
       <c r="E18">
         <v>3</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>916125.05</v>
+        <v>618226.85800000001</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
-      <c r="H18" s="6">
-        <f t="shared" si="4"/>
-        <v>1002325</v>
+      <c r="H18" s="7">
+        <v>676397</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>70</v>
@@ -8830,21 +8814,20 @@
       </c>
       <c r="D19">
         <f t="shared" si="3"/>
-        <v>85549.617999999988</v>
+        <v>56660.497999999992</v>
       </c>
       <c r="E19">
         <v>3</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>909213.38199999998</v>
+        <v>602182.50199999998</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
-      <c r="H19" s="6">
-        <f t="shared" si="4"/>
-        <v>994763</v>
+      <c r="H19" s="7">
+        <v>658843</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>71</v>
@@ -8881,21 +8864,20 @@
       </c>
       <c r="D20">
         <f t="shared" si="3"/>
-        <v>83921.207999999999</v>
+        <v>55902.493999999999</v>
       </c>
       <c r="E20">
         <v>3</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>891906.79200000002</v>
+        <v>594126.50600000005</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
-      <c r="H20" s="6">
-        <f t="shared" si="4"/>
-        <v>975828</v>
+      <c r="H20" s="7">
+        <v>650029</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>72</v>
@@ -8932,21 +8914,20 @@
       </c>
       <c r="D21">
         <f t="shared" si="3"/>
-        <v>81463.757999999987</v>
+        <v>55638.559999999998</v>
       </c>
       <c r="E21">
         <v>3</v>
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>865789.24200000009</v>
+        <v>591321.44000000006</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
-      <c r="H21" s="6">
-        <f t="shared" si="4"/>
-        <v>947253</v>
+      <c r="H21" s="7">
+        <v>646960</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>73</v>
@@ -8965,7 +8946,7 @@
       </c>
       <c r="N21" s="6">
         <f t="shared" si="2"/>
-        <v>3.0000000001164153</v>
+        <v>3</v>
       </c>
       <c r="O21">
         <v>2</v>
@@ -8983,21 +8964,20 @@
       </c>
       <c r="D22">
         <f t="shared" si="3"/>
-        <v>78593.25</v>
+        <v>55485.651999999995</v>
       </c>
       <c r="E22">
         <v>3</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>835281.75</v>
+        <v>589696.348</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
-      <c r="H22" s="6">
-        <f t="shared" si="4"/>
-        <v>913875</v>
+      <c r="H22" s="7">
+        <v>645182</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>74</v>
@@ -9034,21 +9014,20 @@
       </c>
       <c r="D23">
         <f t="shared" si="3"/>
-        <v>65325.202000000012</v>
+        <v>47427.858000000007</v>
       </c>
       <c r="E23">
         <v>3</v>
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>817447.79799999995</v>
+        <v>593489.14199999999</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
-      <c r="H23" s="6">
-        <f t="shared" si="4"/>
-        <v>882773</v>
+      <c r="H23" s="7">
+        <v>640917</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>75</v>
@@ -9085,21 +9064,20 @@
       </c>
       <c r="D24">
         <f t="shared" si="3"/>
-        <v>63496.44000000001</v>
+        <v>46890.988000000005</v>
       </c>
       <c r="E24">
         <v>3</v>
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>794563.55999999994</v>
+        <v>586771.01199999999</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
-      <c r="H24" s="6">
-        <f t="shared" si="4"/>
-        <v>858060</v>
+      <c r="H24" s="7">
+        <v>633662</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>76</v>
@@ -9117,7 +9095,7 @@
         <v>7.4</v>
       </c>
       <c r="N24" s="6">
-        <f t="shared" ref="N24:N63" si="5">SUM(D24:F24)-H24</f>
+        <f t="shared" ref="N24:N63" si="4">SUM(D24:F24)-H24</f>
         <v>3</v>
       </c>
       <c r="O24">
@@ -9136,21 +9114,20 @@
       </c>
       <c r="D25">
         <f t="shared" si="3"/>
-        <v>62418.556000000011</v>
+        <v>46002.692000000003</v>
       </c>
       <c r="E25">
         <v>3</v>
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>781075.4439999999</v>
+        <v>575655.30799999996</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
-      <c r="H25" s="6">
-        <f t="shared" si="4"/>
-        <v>843494</v>
+      <c r="H25" s="7">
+        <v>621658</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>77</v>
@@ -9168,8 +9145,8 @@
         <v>7.4</v>
       </c>
       <c r="N25" s="6">
-        <f t="shared" si="5"/>
-        <v>2.9999999998835847</v>
+        <f t="shared" si="4"/>
+        <v>3</v>
       </c>
       <c r="O25">
         <v>3</v>
@@ -9187,21 +9164,20 @@
       </c>
       <c r="D26">
         <f t="shared" si="3"/>
-        <v>61885.534000000007</v>
+        <v>44830.97600000001</v>
       </c>
       <c r="E26">
         <v>3</v>
       </c>
       <c r="F26">
         <f t="shared" si="1"/>
-        <v>774405.4659999999</v>
+        <v>560993.02399999998</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
-      <c r="H26" s="6">
-        <f t="shared" si="4"/>
-        <v>836291</v>
+      <c r="H26" s="7">
+        <v>605824</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>78</v>
@@ -9219,8 +9195,8 @@
         <v>7.4</v>
       </c>
       <c r="N26" s="6">
-        <f t="shared" si="5"/>
-        <v>2.9999999998835847</v>
+        <f t="shared" si="4"/>
+        <v>3</v>
       </c>
       <c r="O26">
         <v>3</v>
@@ -9238,21 +9214,20 @@
       </c>
       <c r="D27">
         <f t="shared" si="3"/>
-        <v>61515.386000000006</v>
+        <v>43581.486000000004</v>
       </c>
       <c r="E27">
         <v>3</v>
       </c>
       <c r="F27">
         <f t="shared" si="1"/>
-        <v>769773.61399999994</v>
+        <v>545357.51399999997</v>
       </c>
       <c r="G27">
         <v>0</v>
       </c>
-      <c r="H27" s="6">
-        <f t="shared" si="4"/>
-        <v>831289</v>
+      <c r="H27" s="7">
+        <v>588939</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>79</v>
@@ -9270,7 +9245,7 @@
         <v>7.4</v>
       </c>
       <c r="N27" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O27">
@@ -9289,21 +9264,20 @@
       </c>
       <c r="D28">
         <f t="shared" si="3"/>
-        <v>58387.133999999998</v>
+        <v>40618.602999999996</v>
       </c>
       <c r="E28">
         <v>3</v>
       </c>
       <c r="F28">
         <f t="shared" si="1"/>
-        <v>763966.86600000004</v>
+        <v>531474.397</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
-      <c r="H28" s="6">
-        <f t="shared" si="4"/>
-        <v>822354</v>
+      <c r="H28" s="7">
+        <v>572093</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>80</v>
@@ -9321,7 +9295,7 @@
         <v>7.1</v>
       </c>
       <c r="N28" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O28">
@@ -9340,21 +9314,20 @@
       </c>
       <c r="D29">
         <f t="shared" si="3"/>
-        <v>57328.95</v>
+        <v>39321.574999999997</v>
       </c>
       <c r="E29">
         <v>3</v>
       </c>
       <c r="F29">
         <f t="shared" si="1"/>
-        <v>750121.05</v>
+        <v>514503.42500000005</v>
       </c>
       <c r="G29">
         <v>0</v>
       </c>
-      <c r="H29" s="6">
-        <f t="shared" si="4"/>
-        <v>807450</v>
+      <c r="H29" s="7">
+        <v>553825</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>81</v>
@@ -9372,7 +9345,7 @@
         <v>7.1</v>
       </c>
       <c r="N29" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O29">
@@ -9391,21 +9364,20 @@
       </c>
       <c r="D30">
         <f t="shared" si="3"/>
-        <v>55701.842999999993</v>
+        <v>37940.837999999996</v>
       </c>
       <c r="E30">
         <v>3</v>
       </c>
       <c r="F30">
         <f t="shared" si="1"/>
-        <v>728831.15700000001</v>
+        <v>496437.16200000001</v>
       </c>
       <c r="G30">
         <v>0</v>
       </c>
-      <c r="H30" s="6">
-        <f t="shared" si="4"/>
-        <v>784533</v>
+      <c r="H30" s="7">
+        <v>534378</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>82</v>
@@ -9423,7 +9395,7 @@
         <v>7.1</v>
       </c>
       <c r="N30" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O30">
@@ -9442,21 +9414,20 @@
       </c>
       <c r="D31">
         <f t="shared" si="3"/>
-        <v>53690.270999999993</v>
+        <v>36512.814999999995</v>
       </c>
       <c r="E31">
         <v>3</v>
       </c>
       <c r="F31">
         <f t="shared" si="1"/>
-        <v>702510.72900000005</v>
+        <v>477752.185</v>
       </c>
       <c r="G31">
         <v>0</v>
       </c>
-      <c r="H31" s="6">
-        <f t="shared" si="4"/>
-        <v>756201</v>
+      <c r="H31" s="7">
+        <v>514265</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>83</v>
@@ -9474,7 +9445,7 @@
         <v>7.1</v>
       </c>
       <c r="N31" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O31">
@@ -9493,21 +9464,20 @@
       </c>
       <c r="D32">
         <f t="shared" si="3"/>
-        <v>51559.986999999994</v>
+        <v>35054.261999999995</v>
       </c>
       <c r="E32">
         <v>3</v>
       </c>
       <c r="F32">
         <f t="shared" si="1"/>
-        <v>674637.01300000004</v>
+        <v>458667.73800000001</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
-      <c r="H32" s="6">
-        <f t="shared" si="4"/>
-        <v>726197</v>
+      <c r="H32" s="7">
+        <v>493722</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>84</v>
@@ -9525,7 +9495,7 @@
         <v>7.1</v>
       </c>
       <c r="N32" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O32">
@@ -9544,21 +9514,20 @@
       </c>
       <c r="D33">
         <f t="shared" si="3"/>
-        <v>53849.873</v>
+        <v>36446.794999999998</v>
       </c>
       <c r="E33">
         <v>3</v>
       </c>
       <c r="F33">
         <f t="shared" si="1"/>
-        <v>645499.12699999998</v>
+        <v>436888.20499999996</v>
       </c>
       <c r="G33">
         <v>0</v>
       </c>
-      <c r="H33" s="6">
-        <f t="shared" si="4"/>
-        <v>699349</v>
+      <c r="H33" s="7">
+        <v>473335</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>85</v>
@@ -9576,8 +9545,8 @@
         <v>7.7</v>
       </c>
       <c r="N33" s="6">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>2.9999999999417923</v>
       </c>
       <c r="O33">
         <v>5</v>
@@ -9595,21 +9564,20 @@
       </c>
       <c r="D34">
         <f t="shared" si="3"/>
-        <v>52201.072</v>
+        <v>34937.595000000001</v>
       </c>
       <c r="E34">
         <v>3</v>
       </c>
       <c r="F34">
         <f t="shared" si="1"/>
-        <v>625734.92799999996</v>
+        <v>418797.40499999997</v>
       </c>
       <c r="G34">
         <v>0</v>
       </c>
-      <c r="H34" s="6">
-        <f t="shared" si="4"/>
-        <v>677936</v>
+      <c r="H34" s="7">
+        <v>453735</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>86</v>
@@ -9627,7 +9595,7 @@
         <v>7.7</v>
       </c>
       <c r="N34" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O34">
@@ -9646,21 +9614,20 @@
       </c>
       <c r="D35">
         <f t="shared" si="3"/>
-        <v>51118.375</v>
+        <v>33516.406000000003</v>
       </c>
       <c r="E35">
         <v>3</v>
       </c>
       <c r="F35">
         <f t="shared" si="1"/>
-        <v>612756.625</v>
+        <v>401761.59399999998</v>
       </c>
       <c r="G35">
         <v>0</v>
       </c>
-      <c r="H35" s="6">
-        <f t="shared" si="4"/>
-        <v>663875</v>
+      <c r="H35" s="7">
+        <v>435278</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>87</v>
@@ -9678,7 +9645,7 @@
         <v>7.7</v>
       </c>
       <c r="N35" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O35">
@@ -9697,21 +9664,20 @@
       </c>
       <c r="D36">
         <f t="shared" si="3"/>
-        <v>50415.442000000003</v>
+        <v>32160.59</v>
       </c>
       <c r="E36">
         <v>3</v>
       </c>
       <c r="F36">
         <f t="shared" si="1"/>
-        <v>604330.55799999996</v>
+        <v>385509.41</v>
       </c>
       <c r="G36">
         <v>0</v>
       </c>
-      <c r="H36" s="6">
-        <f t="shared" si="4"/>
-        <v>654746</v>
+      <c r="H36" s="7">
+        <v>417670</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>88</v>
@@ -9729,7 +9695,7 @@
         <v>7.7</v>
       </c>
       <c r="N36" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O36">
@@ -9748,21 +9714,20 @@
       </c>
       <c r="D37">
         <f t="shared" si="3"/>
-        <v>49818.923000000003</v>
+        <v>30865.142</v>
       </c>
       <c r="E37">
         <v>3</v>
       </c>
       <c r="F37">
         <f t="shared" si="1"/>
-        <v>597180.07699999993</v>
+        <v>369980.85799999995</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
-      <c r="H37" s="6">
-        <f t="shared" si="4"/>
-        <v>646999</v>
+      <c r="H37" s="7">
+        <v>400846</v>
       </c>
       <c r="I37" s="3" t="s">
         <v>89</v>
@@ -9780,8 +9745,8 @@
         <v>7.7</v>
       </c>
       <c r="N37" s="6">
-        <f t="shared" si="5"/>
-        <v>2.9999999998835847</v>
+        <f t="shared" si="4"/>
+        <v>2.9999999999417923</v>
       </c>
       <c r="O37">
         <v>5</v>
@@ -9799,21 +9764,20 @@
       </c>
       <c r="D38">
         <f t="shared" si="3"/>
-        <v>57362.85</v>
+        <v>34563.599999999999</v>
       </c>
       <c r="E38">
         <v>3</v>
       </c>
       <c r="F38">
         <f t="shared" si="1"/>
-        <v>580002.15</v>
+        <v>349476.4</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
-      <c r="H38" s="6">
-        <f t="shared" si="4"/>
-        <v>637365</v>
+      <c r="H38" s="7">
+        <v>384040</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>90</v>
@@ -9831,7 +9795,7 @@
         <v>9</v>
       </c>
       <c r="N38" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O38">
@@ -9850,21 +9814,20 @@
       </c>
       <c r="D39">
         <f t="shared" si="3"/>
-        <v>56287.89</v>
+        <v>32984.639999999999</v>
       </c>
       <c r="E39">
         <v>3</v>
       </c>
       <c r="F39">
         <f t="shared" si="1"/>
-        <v>569133.11</v>
+        <v>333511.36</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
-      <c r="H39" s="6">
-        <f t="shared" si="4"/>
-        <v>625421</v>
+      <c r="H39" s="7">
+        <v>366496</v>
       </c>
       <c r="I39" s="3" t="s">
         <v>91</v>
@@ -9882,7 +9845,7 @@
         <v>9</v>
       </c>
       <c r="N39" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O39">
@@ -9901,21 +9864,20 @@
       </c>
       <c r="D40">
         <f t="shared" si="3"/>
-        <v>54860.49</v>
+        <v>31308.3</v>
       </c>
       <c r="E40">
         <v>3</v>
       </c>
       <c r="F40">
         <f t="shared" si="1"/>
-        <v>554700.51</v>
+        <v>316561.7</v>
       </c>
       <c r="G40">
         <v>0</v>
       </c>
-      <c r="H40" s="6">
-        <f t="shared" si="4"/>
-        <v>609561</v>
+      <c r="H40" s="7">
+        <v>347870</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>92</v>
@@ -9933,7 +9895,7 @@
         <v>9</v>
       </c>
       <c r="N40" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O40">
@@ -9952,21 +9914,20 @@
       </c>
       <c r="D41">
         <f t="shared" si="3"/>
-        <v>53154</v>
+        <v>29610.719999999998</v>
       </c>
       <c r="E41">
         <v>3</v>
       </c>
       <c r="F41">
         <f t="shared" si="1"/>
-        <v>537446</v>
+        <v>299397.28000000003</v>
       </c>
       <c r="G41">
         <v>0</v>
       </c>
-      <c r="H41" s="6">
-        <f t="shared" si="4"/>
-        <v>590600</v>
+      <c r="H41" s="7">
+        <v>329008</v>
       </c>
       <c r="I41" s="3" t="s">
         <v>93</v>
@@ -9984,7 +9945,7 @@
         <v>9</v>
       </c>
       <c r="N41" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O41">
@@ -10003,21 +9964,20 @@
       </c>
       <c r="D42">
         <f t="shared" si="3"/>
-        <v>51376.409999999996</v>
+        <v>27876.87</v>
       </c>
       <c r="E42">
         <v>3</v>
       </c>
       <c r="F42">
         <f t="shared" si="1"/>
-        <v>519472.59</v>
+        <v>281866.13</v>
       </c>
       <c r="G42">
         <v>0</v>
       </c>
-      <c r="H42" s="6">
-        <f t="shared" si="4"/>
-        <v>570849</v>
+      <c r="H42" s="7">
+        <v>309743</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>94</v>
@@ -10035,7 +9995,7 @@
         <v>9</v>
       </c>
       <c r="N42" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O42">
@@ -10054,21 +10014,20 @@
       </c>
       <c r="D43">
         <f t="shared" si="3"/>
-        <v>52364.855000000003</v>
+        <v>27774.295000000002</v>
       </c>
       <c r="E43">
         <v>3</v>
       </c>
       <c r="F43">
         <f t="shared" si="1"/>
-        <v>498844.14500000002</v>
+        <v>264586.70500000002</v>
       </c>
       <c r="G43">
         <v>0</v>
       </c>
-      <c r="H43" s="6">
-        <f t="shared" si="4"/>
-        <v>551209</v>
+      <c r="H43" s="7">
+        <v>292361</v>
       </c>
       <c r="I43" s="3" t="s">
         <v>95</v>
@@ -10086,7 +10045,7 @@
         <v>9.5</v>
       </c>
       <c r="N43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O43">
@@ -10105,21 +10064,20 @@
       </c>
       <c r="D44">
         <f t="shared" si="3"/>
-        <v>50386.004999999997</v>
+        <v>26588.79</v>
       </c>
       <c r="E44">
         <v>3</v>
       </c>
       <c r="F44">
         <f t="shared" si="1"/>
-        <v>479992.995</v>
+        <v>253293.21000000002</v>
       </c>
       <c r="G44">
         <v>0</v>
       </c>
-      <c r="H44" s="6">
-        <f t="shared" si="4"/>
-        <v>530379</v>
+      <c r="H44" s="7">
+        <v>279882</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>96</v>
@@ -10137,7 +10095,7 @@
         <v>9.5</v>
       </c>
       <c r="N44" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O44">
@@ -10156,21 +10114,20 @@
       </c>
       <c r="D45">
         <f t="shared" si="3"/>
-        <v>48322.224999999999</v>
+        <v>26024.014999999999</v>
       </c>
       <c r="E45">
         <v>3</v>
       </c>
       <c r="F45">
         <f t="shared" si="1"/>
-        <v>460332.77500000002</v>
+        <v>247912.98500000002</v>
       </c>
       <c r="G45">
         <v>0</v>
       </c>
-      <c r="H45" s="6">
-        <f t="shared" si="4"/>
-        <v>508655</v>
+      <c r="H45" s="7">
+        <v>273937</v>
       </c>
       <c r="I45" s="3" t="s">
         <v>97</v>
@@ -10188,7 +10145,7 @@
         <v>9.5</v>
       </c>
       <c r="N45" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O45">
@@ -10207,21 +10164,20 @@
       </c>
       <c r="D46">
         <f t="shared" si="3"/>
-        <v>46212.18</v>
+        <v>25914.764999999999</v>
       </c>
       <c r="E46">
         <v>3</v>
       </c>
       <c r="F46">
         <f t="shared" si="1"/>
-        <v>440231.82</v>
+        <v>246872.23500000002</v>
       </c>
       <c r="G46">
         <v>0</v>
       </c>
-      <c r="H46" s="6">
-        <f t="shared" si="4"/>
-        <v>486444</v>
+      <c r="H46" s="7">
+        <v>272787</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>98</v>
@@ -10239,7 +10195,7 @@
         <v>9.5</v>
       </c>
       <c r="N46" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O46">
@@ -10258,21 +10214,20 @@
       </c>
       <c r="D47">
         <f t="shared" si="3"/>
-        <v>44076.01</v>
+        <v>26038.075000000001</v>
       </c>
       <c r="E47">
         <v>3</v>
       </c>
       <c r="F47">
         <f t="shared" si="1"/>
-        <v>419881.99</v>
+        <v>248046.92500000002</v>
       </c>
       <c r="G47">
         <v>0</v>
       </c>
-      <c r="H47" s="6">
-        <f t="shared" si="4"/>
-        <v>463958</v>
+      <c r="H47" s="7">
+        <v>274085</v>
       </c>
       <c r="I47" s="3" t="s">
         <v>99</v>
@@ -10290,7 +10245,7 @@
         <v>9.5</v>
       </c>
       <c r="N47" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O47">
@@ -10309,21 +10264,20 @@
       </c>
       <c r="D48">
         <f t="shared" si="3"/>
-        <v>40642.932000000001</v>
+        <v>25247.928</v>
       </c>
       <c r="E48">
         <v>3</v>
       </c>
       <c r="F48">
         <f t="shared" si="1"/>
-        <v>401128.06799999997</v>
+        <v>249186.07199999999</v>
       </c>
       <c r="G48">
         <v>0</v>
       </c>
-      <c r="H48" s="6">
-        <f t="shared" si="4"/>
-        <v>441771</v>
+      <c r="H48" s="7">
+        <v>274434</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>100</v>
@@ -10341,7 +10295,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="N48" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O48">
@@ -10360,21 +10314,20 @@
       </c>
       <c r="D49">
         <f t="shared" si="3"/>
-        <v>38688.300000000003</v>
+        <v>25017.007999999998</v>
       </c>
       <c r="E49">
         <v>3</v>
       </c>
       <c r="F49">
         <f t="shared" si="1"/>
-        <v>381836.69999999995</v>
+        <v>246906.99199999997</v>
       </c>
       <c r="G49">
         <v>0</v>
       </c>
-      <c r="H49" s="6">
-        <f t="shared" si="4"/>
-        <v>420525</v>
+      <c r="H49" s="7">
+        <v>271924</v>
       </c>
       <c r="I49" s="3" t="s">
         <v>101</v>
@@ -10392,7 +10345,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="N49" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.9999999999417923</v>
       </c>
       <c r="O49">
@@ -10411,21 +10364,20 @@
       </c>
       <c r="D50">
         <f t="shared" si="3"/>
-        <v>36852.716</v>
+        <v>24339.887999999999</v>
       </c>
       <c r="E50">
         <v>3</v>
       </c>
       <c r="F50">
         <f t="shared" si="1"/>
-        <v>363720.28399999999</v>
+        <v>240224.11199999996</v>
       </c>
       <c r="G50">
         <v>0</v>
       </c>
-      <c r="H50" s="6">
-        <f t="shared" si="4"/>
-        <v>400573</v>
+      <c r="H50" s="7">
+        <v>264564</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>102</v>
@@ -10443,8 +10395,8 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="N50" s="6">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>2.9999999999417923</v>
       </c>
       <c r="O50">
         <v>8</v>
@@ -10462,21 +10414,20 @@
       </c>
       <c r="D51">
         <f t="shared" si="3"/>
-        <v>35114.468000000001</v>
+        <v>23329.543999999998</v>
       </c>
       <c r="E51">
         <v>3</v>
       </c>
       <c r="F51">
         <f t="shared" si="1"/>
-        <v>346564.53199999995</v>
+        <v>230252.45599999998</v>
       </c>
       <c r="G51">
         <v>0</v>
       </c>
-      <c r="H51" s="6">
-        <f t="shared" si="4"/>
-        <v>381679</v>
+      <c r="H51" s="7">
+        <v>253582</v>
       </c>
       <c r="I51" s="3" t="s">
         <v>103</v>
@@ -10494,8 +10445,8 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="N51" s="6">
-        <f t="shared" si="5"/>
-        <v>2.9999999999417923</v>
+        <f t="shared" si="4"/>
+        <v>2.9999999999708962</v>
       </c>
       <c r="O51">
         <v>8</v>
@@ -10513,21 +10464,20 @@
       </c>
       <c r="D52">
         <f t="shared" si="3"/>
-        <v>33466.748</v>
+        <v>22225.912</v>
       </c>
       <c r="E52">
         <v>3</v>
       </c>
       <c r="F52">
         <f t="shared" si="1"/>
-        <v>330302.25199999998</v>
+        <v>219360.08799999999</v>
       </c>
       <c r="G52">
         <v>0</v>
       </c>
-      <c r="H52" s="6">
-        <f t="shared" si="4"/>
-        <v>363769</v>
+      <c r="H52" s="7">
+        <v>241586</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>104</v>
@@ -10545,7 +10495,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="N52" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O52">
@@ -10564,21 +10514,20 @@
       </c>
       <c r="D53">
         <f t="shared" si="3"/>
-        <v>37376.100000000006</v>
+        <v>24933.960000000003</v>
       </c>
       <c r="E53">
         <v>3</v>
       </c>
       <c r="F53">
         <f t="shared" si="1"/>
-        <v>308698.90000000002</v>
+        <v>205936.04</v>
       </c>
       <c r="G53">
         <v>0</v>
       </c>
-      <c r="H53" s="6">
-        <f t="shared" si="4"/>
-        <v>346075</v>
+      <c r="H53" s="7">
+        <v>230870</v>
       </c>
       <c r="I53" s="3" t="s">
         <v>105</v>
@@ -10596,7 +10545,7 @@
         <v>10.8</v>
       </c>
       <c r="N53" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O53">
@@ -10615,21 +10564,20 @@
       </c>
       <c r="D54">
         <f t="shared" si="3"/>
-        <v>35406.504000000001</v>
+        <v>23952.240000000002</v>
       </c>
       <c r="E54">
         <v>3</v>
       </c>
       <c r="F54">
         <f t="shared" si="1"/>
-        <v>292431.49599999998</v>
+        <v>197827.76</v>
       </c>
       <c r="G54">
         <v>0</v>
       </c>
-      <c r="H54" s="6">
-        <f t="shared" si="4"/>
-        <v>327838</v>
+      <c r="H54" s="7">
+        <v>221780</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>106</v>
@@ -10647,7 +10595,7 @@
         <v>10.8</v>
       </c>
       <c r="N54" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O54">
@@ -10666,21 +10614,20 @@
       </c>
       <c r="D55">
         <f t="shared" si="3"/>
-        <v>33336.684000000001</v>
+        <v>23242.680000000004</v>
       </c>
       <c r="E55">
         <v>3</v>
       </c>
       <c r="F55">
         <f t="shared" si="1"/>
-        <v>275336.31599999999</v>
+        <v>191967.32</v>
       </c>
       <c r="G55">
         <v>0</v>
       </c>
-      <c r="H55" s="6">
-        <f t="shared" si="4"/>
-        <v>308673</v>
+      <c r="H55" s="7">
+        <v>215210</v>
       </c>
       <c r="I55" s="3" t="s">
         <v>107</v>
@@ -10698,7 +10645,7 @@
         <v>10.8</v>
       </c>
       <c r="N55" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O55">
@@ -10717,21 +10664,20 @@
       </c>
       <c r="D56">
         <f t="shared" si="3"/>
-        <v>31241.592000000004</v>
+        <v>22735.944000000003</v>
       </c>
       <c r="E56">
         <v>3</v>
       </c>
       <c r="F56">
         <f t="shared" si="1"/>
-        <v>258032.408</v>
+        <v>187782.05600000001</v>
       </c>
       <c r="G56">
         <v>0</v>
       </c>
-      <c r="H56" s="6">
-        <f t="shared" si="4"/>
-        <v>289274</v>
+      <c r="H56" s="7">
+        <v>210518</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>108</v>
@@ -10749,7 +10695,7 @@
         <v>10.8</v>
       </c>
       <c r="N56" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O56">
@@ -10768,21 +10714,20 @@
       </c>
       <c r="D57">
         <f t="shared" si="3"/>
-        <v>29106.216000000004</v>
+        <v>22336.776000000002</v>
       </c>
       <c r="E57">
         <v>3</v>
       </c>
       <c r="F57">
         <f t="shared" si="1"/>
-        <v>240395.78400000001</v>
+        <v>184485.22400000002</v>
       </c>
       <c r="G57">
         <v>0</v>
       </c>
-      <c r="H57" s="6">
-        <f t="shared" si="4"/>
-        <v>269502</v>
+      <c r="H57" s="7">
+        <v>206822</v>
       </c>
       <c r="I57" s="3" t="s">
         <v>109</v>
@@ -10800,8 +10745,8 @@
         <v>10.8</v>
       </c>
       <c r="N57" s="6">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>3.0000000000291038</v>
       </c>
       <c r="O57">
         <v>9</v>
@@ -10819,21 +10764,20 @@
       </c>
       <c r="D58">
         <f t="shared" si="3"/>
-        <v>27151.416000000005</v>
+        <v>21859.524000000001</v>
       </c>
       <c r="E58">
         <v>3</v>
       </c>
       <c r="F58">
         <f t="shared" si="1"/>
-        <v>224250.584</v>
+        <v>180543.476</v>
       </c>
       <c r="G58">
         <v>0</v>
       </c>
-      <c r="H58" s="6">
-        <f t="shared" si="4"/>
-        <v>251402</v>
+      <c r="H58" s="7">
+        <v>202403</v>
       </c>
       <c r="I58" s="2" t="s">
         <v>110</v>
@@ -10851,7 +10795,7 @@
         <v>10.8</v>
       </c>
       <c r="N58" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O58">
@@ -10870,21 +10814,20 @@
       </c>
       <c r="D59">
         <f t="shared" si="3"/>
-        <v>25662.312000000002</v>
+        <v>21178.152000000002</v>
       </c>
       <c r="E59">
         <v>3</v>
       </c>
       <c r="F59">
         <f t="shared" si="1"/>
-        <v>211951.68799999999</v>
+        <v>174915.848</v>
       </c>
       <c r="G59">
         <v>0</v>
       </c>
-      <c r="H59" s="6">
-        <f t="shared" si="4"/>
-        <v>237614</v>
+      <c r="H59" s="7">
+        <v>196094</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>111</v>
@@ -10902,7 +10845,7 @@
         <v>10.8</v>
       </c>
       <c r="N59" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O59">
@@ -10921,21 +10864,20 @@
       </c>
       <c r="D60">
         <f t="shared" si="3"/>
-        <v>24787.404000000002</v>
+        <v>20165.760000000002</v>
       </c>
       <c r="E60">
         <v>3</v>
       </c>
       <c r="F60">
         <f t="shared" si="1"/>
-        <v>204725.59599999999</v>
+        <v>166554.23999999999</v>
       </c>
       <c r="G60">
         <v>0</v>
       </c>
-      <c r="H60" s="6">
-        <f t="shared" si="4"/>
-        <v>229513</v>
+      <c r="H60" s="7">
+        <v>186720</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>112</v>
@@ -10953,7 +10895,7 @@
         <v>10.8</v>
       </c>
       <c r="N60" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O60">
@@ -10972,21 +10914,20 @@
       </c>
       <c r="D61">
         <f t="shared" si="3"/>
-        <v>24360.048000000003</v>
+        <v>18899.676000000003</v>
       </c>
       <c r="E61">
         <v>3</v>
       </c>
       <c r="F61">
         <f t="shared" si="1"/>
-        <v>201195.95199999999</v>
+        <v>156097.32399999999</v>
       </c>
       <c r="G61">
         <v>0</v>
       </c>
-      <c r="H61" s="6">
-        <f t="shared" si="4"/>
-        <v>225556</v>
+      <c r="H61" s="7">
+        <v>174997</v>
       </c>
       <c r="I61" s="3" t="s">
         <v>113</v>
@@ -11004,7 +10945,7 @@
         <v>10.8</v>
       </c>
       <c r="N61" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O61">
@@ -11023,21 +10964,20 @@
       </c>
       <c r="D62">
         <f t="shared" si="3"/>
-        <v>24155.712000000003</v>
+        <v>17462.304000000004</v>
       </c>
       <c r="E62">
         <v>3</v>
       </c>
       <c r="F62">
         <f t="shared" si="1"/>
-        <v>199508.288</v>
+        <v>144225.696</v>
       </c>
       <c r="G62">
         <v>0</v>
       </c>
-      <c r="H62" s="6">
-        <f t="shared" si="4"/>
-        <v>223664</v>
+      <c r="H62" s="7">
+        <v>161688</v>
       </c>
       <c r="I62" s="2" t="s">
         <v>114</v>
@@ -11055,7 +10995,7 @@
         <v>10.8</v>
       </c>
       <c r="N62" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O62">
@@ -11074,21 +11014,20 @@
       </c>
       <c r="D63">
         <f>(M63/100)*H63</f>
-        <v>193802.02560000005</v>
+        <v>142033.60800000001</v>
       </c>
       <c r="E63">
         <v>3</v>
       </c>
       <c r="F63">
         <f t="shared" si="1"/>
-        <v>1600661.1744000001</v>
+        <v>1173092.392</v>
       </c>
       <c r="G63">
         <v>0</v>
       </c>
-      <c r="H63" s="6">
-        <f t="shared" si="4"/>
-        <v>1794463.2000000002</v>
+      <c r="H63" s="7">
+        <v>1315126</v>
       </c>
       <c r="I63" s="3" t="s">
         <v>115</v>
@@ -11106,7 +11045,7 @@
         <v>10.8</v>
       </c>
       <c r="N63" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O63">
@@ -11125,21 +11064,20 @@
       </c>
       <c r="D64">
         <f>(M64/100)*H64</f>
-        <v>144133.55352000002</v>
+        <v>59480.568000000007</v>
       </c>
       <c r="E64">
         <v>3</v>
       </c>
       <c r="F64">
         <f t="shared" si="1"/>
-        <v>1190436.3864799999</v>
+        <v>491265.43200000003</v>
       </c>
       <c r="G64">
         <v>0</v>
       </c>
-      <c r="H64" s="6">
-        <f t="shared" si="4"/>
-        <v>1334569.94</v>
+      <c r="H64" s="7">
+        <v>550746</v>
       </c>
       <c r="I64" t="s">
         <v>154</v>
@@ -11195,7 +11133,7 @@
   <dimension ref="A1:F109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M47" sqref="M47"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13389,8 +13327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE7DAD58-4E64-A742-BDF7-21365FC7807C}">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="P55" sqref="P55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13435,16 +13373,16 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>366840.0675</v>
+        <v>394858.95750000002</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>3</v>
       </c>
       <c r="F2">
-        <v>112689.4325</v>
+        <v>121296.5425</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -13467,7 +13405,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>366840.0675</v>
+        <v>383511.33</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -13476,7 +13414,7 @@
         <v>3</v>
       </c>
       <c r="F3">
-        <v>112689.4325</v>
+        <v>117810.67</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -13499,7 +13437,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>703150.51500000001</v>
+        <v>767022.66</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -13508,7 +13446,7 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>216000.48499999999</v>
+        <v>235621.34</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -13531,7 +13469,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>712497.28500000003</v>
+        <v>745344.09</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -13540,7 +13478,7 @@
         <v>3</v>
       </c>
       <c r="F5">
-        <v>218871.715</v>
+        <v>228961.90999999997</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -13563,7 +13501,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>739210.32000000007</v>
+        <v>720550.44000000006</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -13572,7 +13510,7 @@
         <v>3</v>
       </c>
       <c r="F6">
-        <v>227077.68</v>
+        <v>221345.56</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -13595,7 +13533,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>724268.34</v>
+        <v>692695.26</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -13604,7 +13542,7 @@
         <v>3</v>
       </c>
       <c r="F7">
-        <v>222487.65999999997</v>
+        <v>212788.74</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -13627,7 +13565,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>382644.50400000002</v>
+        <v>350178.984</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -13636,7 +13574,7 @@
         <v>3</v>
       </c>
       <c r="F8">
-        <v>569207.49599999993</v>
+        <v>520913.016</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -13659,7 +13597,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>383901.96</v>
+        <v>338841.37800000003</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -13668,7 +13606,7 @@
         <v>3</v>
       </c>
       <c r="F9">
-        <v>571078.03999999992</v>
+        <v>504047.62199999997</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -13691,7 +13629,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>386153.96400000004</v>
+        <v>331579.24800000002</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -13700,7 +13638,7 @@
         <v>3</v>
       </c>
       <c r="F10">
-        <v>574428.03599999996</v>
+        <v>493244.75199999998</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -13723,7 +13661,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>388522.14600000001</v>
+        <v>327330.51</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -13732,7 +13670,7 @@
         <v>3</v>
       </c>
       <c r="F11">
-        <v>577950.85399999993</v>
+        <v>486924.49</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -13755,7 +13693,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>391383.984</v>
+        <v>324290.98800000001</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -13764,7 +13702,7 @@
         <v>3</v>
       </c>
       <c r="F12">
-        <v>582208.01599999995</v>
+        <v>482403.01199999999</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -13787,7 +13725,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>170117.12800000003</v>
+        <v>137730.49000000002</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -13796,7 +13734,7 @@
         <v>3</v>
       </c>
       <c r="F13">
-        <v>813218.87200000009</v>
+        <v>658399.51</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -13819,7 +13757,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>171482.27100000001</v>
+        <v>134983.42300000001</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -13828,7 +13766,7 @@
         <v>3</v>
       </c>
       <c r="F14">
-        <v>819744.72900000005</v>
+        <v>645267.57700000005</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -13851,7 +13789,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>173080.27200000003</v>
+        <v>130949.92800000001</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -13860,7 +13798,7 @@
         <v>3</v>
       </c>
       <c r="F15">
-        <v>827383.72800000012</v>
+        <v>625986.07200000004</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -13883,7 +13821,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>174552.67500000002</v>
+        <v>126140.18200000002</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -13892,7 +13830,7 @@
         <v>3</v>
       </c>
       <c r="F16">
-        <v>834422.32500000007</v>
+        <v>602993.81800000009</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -13915,7 +13853,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>175646.38100000002</v>
+        <v>121213.31500000002</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -13924,7 +13862,7 @@
         <v>3</v>
       </c>
       <c r="F17">
-        <v>839650.61900000006</v>
+        <v>579441.68500000006</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -13947,7 +13885,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>86199.95</v>
+        <v>58170.141999999993</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -13956,7 +13894,7 @@
         <v>3</v>
       </c>
       <c r="F18">
-        <v>916125.05</v>
+        <v>618226.85800000001</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -13979,7 +13917,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <v>85549.617999999988</v>
+        <v>56660.497999999992</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -13988,7 +13926,7 @@
         <v>3</v>
       </c>
       <c r="F19">
-        <v>909213.38199999998</v>
+        <v>602182.50199999998</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -14011,7 +13949,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>83921.207999999999</v>
+        <v>55902.493999999999</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -14020,7 +13958,7 @@
         <v>3</v>
       </c>
       <c r="F20">
-        <v>891906.79200000002</v>
+        <v>594126.50600000005</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -14043,7 +13981,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>81463.757999999987</v>
+        <v>55638.559999999998</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -14052,7 +13990,7 @@
         <v>3</v>
       </c>
       <c r="F21">
-        <v>865789.24200000009</v>
+        <v>591321.44000000006</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -14075,7 +14013,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>78593.25</v>
+        <v>55485.651999999995</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -14084,7 +14022,7 @@
         <v>3</v>
       </c>
       <c r="F22">
-        <v>835281.75</v>
+        <v>589696.348</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -14107,7 +14045,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <v>65325.202000000012</v>
+        <v>47427.858000000007</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -14116,7 +14054,7 @@
         <v>3</v>
       </c>
       <c r="F23">
-        <v>817447.79799999995</v>
+        <v>593489.14199999999</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -14139,7 +14077,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>63496.44000000001</v>
+        <v>46890.988000000005</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -14148,7 +14086,7 @@
         <v>3</v>
       </c>
       <c r="F24">
-        <v>794563.55999999994</v>
+        <v>586771.01199999999</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -14171,7 +14109,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>62418.556000000011</v>
+        <v>46002.692000000003</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -14180,7 +14118,7 @@
         <v>3</v>
       </c>
       <c r="F25">
-        <v>781075.4439999999</v>
+        <v>575655.30799999996</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -14203,7 +14141,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>61885.534000000007</v>
+        <v>44830.97600000001</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -14212,7 +14150,7 @@
         <v>3</v>
       </c>
       <c r="F26">
-        <v>774405.4659999999</v>
+        <v>560993.02399999998</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -14235,7 +14173,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <v>61515.386000000006</v>
+        <v>43581.486000000004</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -14244,7 +14182,7 @@
         <v>3</v>
       </c>
       <c r="F27">
-        <v>769773.61399999994</v>
+        <v>545357.51399999997</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -14267,7 +14205,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <v>58387.133999999998</v>
+        <v>40618.602999999996</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -14276,7 +14214,7 @@
         <v>3</v>
       </c>
       <c r="F28">
-        <v>763966.86600000004</v>
+        <v>531474.397</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -14299,7 +14237,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <v>57328.95</v>
+        <v>39321.574999999997</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -14308,7 +14246,7 @@
         <v>3</v>
       </c>
       <c r="F29">
-        <v>750121.05</v>
+        <v>514503.42500000005</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -14331,7 +14269,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <v>55701.842999999993</v>
+        <v>37940.837999999996</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -14340,7 +14278,7 @@
         <v>3</v>
       </c>
       <c r="F30">
-        <v>728831.15700000001</v>
+        <v>496437.16200000001</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -14363,7 +14301,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <v>53690.270999999993</v>
+        <v>36512.814999999995</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -14372,7 +14310,7 @@
         <v>3</v>
       </c>
       <c r="F31">
-        <v>702510.72900000005</v>
+        <v>477752.185</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -14395,7 +14333,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <v>51559.986999999994</v>
+        <v>35054.261999999995</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -14404,7 +14342,7 @@
         <v>3</v>
       </c>
       <c r="F32">
-        <v>674637.01300000004</v>
+        <v>458667.73800000001</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -14427,7 +14365,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <v>53849.873</v>
+        <v>36446.794999999998</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -14436,7 +14374,7 @@
         <v>3</v>
       </c>
       <c r="F33">
-        <v>645499.12699999998</v>
+        <v>436888.20499999996</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -14459,7 +14397,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <v>52201.072</v>
+        <v>34937.595000000001</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -14468,7 +14406,7 @@
         <v>3</v>
       </c>
       <c r="F34">
-        <v>625734.92799999996</v>
+        <v>418797.40499999997</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -14491,7 +14429,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <v>51118.375</v>
+        <v>33516.406000000003</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -14500,7 +14438,7 @@
         <v>3</v>
       </c>
       <c r="F35">
-        <v>612756.625</v>
+        <v>401761.59399999998</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -14523,7 +14461,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <v>50415.442000000003</v>
+        <v>32160.59</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -14532,7 +14470,7 @@
         <v>3</v>
       </c>
       <c r="F36">
-        <v>604330.55799999996</v>
+        <v>385509.41</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -14555,7 +14493,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <v>49818.923000000003</v>
+        <v>30865.142</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -14564,7 +14502,7 @@
         <v>3</v>
       </c>
       <c r="F37">
-        <v>597180.07699999993</v>
+        <v>369980.85799999995</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -14587,7 +14525,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <v>57362.85</v>
+        <v>34563.599999999999</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -14596,7 +14534,7 @@
         <v>3</v>
       </c>
       <c r="F38">
-        <v>580002.15</v>
+        <v>349476.4</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -14619,7 +14557,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <v>56287.89</v>
+        <v>32984.639999999999</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -14628,7 +14566,7 @@
         <v>3</v>
       </c>
       <c r="F39">
-        <v>569133.11</v>
+        <v>333511.36</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -14651,7 +14589,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <v>54860.49</v>
+        <v>31308.3</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -14660,7 +14598,7 @@
         <v>3</v>
       </c>
       <c r="F40">
-        <v>554700.51</v>
+        <v>316561.7</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -14683,7 +14621,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>53154</v>
+        <v>29610.719999999998</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -14692,7 +14630,7 @@
         <v>3</v>
       </c>
       <c r="F41">
-        <v>537446</v>
+        <v>299397.28000000003</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -14715,7 +14653,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <v>51376.409999999996</v>
+        <v>27876.87</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -14724,7 +14662,7 @@
         <v>3</v>
       </c>
       <c r="F42">
-        <v>519472.59</v>
+        <v>281866.13</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -14747,7 +14685,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <v>52364.855000000003</v>
+        <v>27774.295000000002</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -14756,7 +14694,7 @@
         <v>3</v>
       </c>
       <c r="F43">
-        <v>498844.14500000002</v>
+        <v>264586.70500000002</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -14779,7 +14717,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <v>50386.004999999997</v>
+        <v>26588.79</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -14788,7 +14726,7 @@
         <v>3</v>
       </c>
       <c r="F44">
-        <v>479992.995</v>
+        <v>253293.21000000002</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -14811,7 +14749,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <v>48322.224999999999</v>
+        <v>26024.014999999999</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -14820,7 +14758,7 @@
         <v>3</v>
       </c>
       <c r="F45">
-        <v>460332.77500000002</v>
+        <v>247912.98500000002</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -14843,7 +14781,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <v>46212.18</v>
+        <v>25914.764999999999</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -14852,7 +14790,7 @@
         <v>3</v>
       </c>
       <c r="F46">
-        <v>440231.82</v>
+        <v>246872.23500000002</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -14875,7 +14813,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <v>44076.01</v>
+        <v>26038.075000000001</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -14884,7 +14822,7 @@
         <v>3</v>
       </c>
       <c r="F47">
-        <v>419881.99</v>
+        <v>248046.92500000002</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -14907,7 +14845,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <v>40642.932000000001</v>
+        <v>25247.928</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -14916,7 +14854,7 @@
         <v>3</v>
       </c>
       <c r="F48">
-        <v>401128.06799999997</v>
+        <v>249186.07199999999</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -14939,7 +14877,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <v>38688.300000000003</v>
+        <v>25017.007999999998</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -14948,7 +14886,7 @@
         <v>3</v>
       </c>
       <c r="F49">
-        <v>381836.69999999995</v>
+        <v>246906.99199999997</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -14971,7 +14909,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <v>36852.716</v>
+        <v>24339.887999999999</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -14980,7 +14918,7 @@
         <v>3</v>
       </c>
       <c r="F50">
-        <v>363720.28399999999</v>
+        <v>240224.11199999996</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -15003,7 +14941,7 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <v>35114.468000000001</v>
+        <v>23329.543999999998</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -15012,7 +14950,7 @@
         <v>3</v>
       </c>
       <c r="F51">
-        <v>346564.53199999995</v>
+        <v>230252.45599999998</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -15035,7 +14973,7 @@
         <v>0</v>
       </c>
       <c r="C52">
-        <v>33466.748</v>
+        <v>22225.912</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -15044,7 +14982,7 @@
         <v>3</v>
       </c>
       <c r="F52">
-        <v>330302.25199999998</v>
+        <v>219360.08799999999</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -15067,7 +15005,7 @@
         <v>0</v>
       </c>
       <c r="C53">
-        <v>37376.100000000006</v>
+        <v>24933.960000000003</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -15076,7 +15014,7 @@
         <v>3</v>
       </c>
       <c r="F53">
-        <v>308698.90000000002</v>
+        <v>205936.04</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -15099,7 +15037,7 @@
         <v>0</v>
       </c>
       <c r="C54">
-        <v>35406.504000000001</v>
+        <v>23952.240000000002</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -15108,7 +15046,7 @@
         <v>3</v>
       </c>
       <c r="F54">
-        <v>292431.49599999998</v>
+        <v>197827.76</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -15131,7 +15069,7 @@
         <v>0</v>
       </c>
       <c r="C55">
-        <v>33336.684000000001</v>
+        <v>23242.680000000004</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -15140,7 +15078,7 @@
         <v>3</v>
       </c>
       <c r="F55">
-        <v>275336.31599999999</v>
+        <v>191967.32</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -15163,7 +15101,7 @@
         <v>0</v>
       </c>
       <c r="C56">
-        <v>31241.592000000004</v>
+        <v>22735.944000000003</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -15172,7 +15110,7 @@
         <v>3</v>
       </c>
       <c r="F56">
-        <v>258032.408</v>
+        <v>187782.05600000001</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -15195,7 +15133,7 @@
         <v>0</v>
       </c>
       <c r="C57">
-        <v>29106.216000000004</v>
+        <v>22336.776000000002</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -15204,7 +15142,7 @@
         <v>3</v>
       </c>
       <c r="F57">
-        <v>240395.78400000001</v>
+        <v>184485.22400000002</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -15227,7 +15165,7 @@
         <v>0</v>
       </c>
       <c r="C58">
-        <v>27151.416000000005</v>
+        <v>21859.524000000001</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -15236,7 +15174,7 @@
         <v>3</v>
       </c>
       <c r="F58">
-        <v>224250.584</v>
+        <v>180543.476</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -15259,7 +15197,7 @@
         <v>0</v>
       </c>
       <c r="C59">
-        <v>25662.312000000002</v>
+        <v>21178.152000000002</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -15268,7 +15206,7 @@
         <v>3</v>
       </c>
       <c r="F59">
-        <v>211951.68799999999</v>
+        <v>174915.848</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -15291,7 +15229,7 @@
         <v>0</v>
       </c>
       <c r="C60">
-        <v>24787.404000000002</v>
+        <v>20165.760000000002</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -15300,7 +15238,7 @@
         <v>3</v>
       </c>
       <c r="F60">
-        <v>204725.59599999999</v>
+        <v>166554.23999999999</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -15323,7 +15261,7 @@
         <v>0</v>
       </c>
       <c r="C61">
-        <v>24360.048000000003</v>
+        <v>18899.676000000003</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -15332,7 +15270,7 @@
         <v>3</v>
       </c>
       <c r="F61">
-        <v>201195.95199999999</v>
+        <v>156097.32399999999</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -15355,7 +15293,7 @@
         <v>0</v>
       </c>
       <c r="C62">
-        <v>24155.712000000003</v>
+        <v>17462.304000000004</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -15364,7 +15302,7 @@
         <v>3</v>
       </c>
       <c r="F62">
-        <v>199508.288</v>
+        <v>144225.696</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -15387,7 +15325,7 @@
         <v>0</v>
       </c>
       <c r="C63">
-        <v>193802.02560000005</v>
+        <v>142033.60800000001</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -15396,7 +15334,7 @@
         <v>3</v>
       </c>
       <c r="F63">
-        <v>1600661.1744000001</v>
+        <v>1173092.392</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -15419,7 +15357,7 @@
         <v>0</v>
       </c>
       <c r="C64">
-        <v>144133.55352000002</v>
+        <v>59480.568000000007</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -15428,7 +15366,7 @@
         <v>3</v>
       </c>
       <c r="F64">
-        <v>1190436.3864799999</v>
+        <v>491265.43200000003</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -15452,8 +15390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F657C2F3-B3C3-AD44-B220-FE5C72CA33E4}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
new Ptrans from script
</commit_message>
<xml_diff>
--- a/parameters/DataWorkbookRubella.xlsx
+++ b/parameters/DataWorkbookRubella.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taahir/Downloads/RubellaNew/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84A237F-5E6C-D34A-92D8-A5CB5B124DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82DA0D9-1B70-0F44-8701-330A390BA4B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="coverage_table " sheetId="1" r:id="rId1"/>
     <sheet name="age_ref" sheetId="2" r:id="rId2"/>
     <sheet name="Initial_conditions" sheetId="3" r:id="rId3"/>
     <sheet name="Initial_conditions_small" sheetId="4" r:id="rId4"/>
-    <sheet name="init_cond_old" sheetId="5" r:id="rId5"/>
-    <sheet name="init_cond" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId7"/>
-    <sheet name="old_cond" sheetId="7" r:id="rId8"/>
-    <sheet name="Original_Prev" sheetId="8" r:id="rId9"/>
+    <sheet name="init_test" sheetId="10" r:id="rId5"/>
+    <sheet name="init_cond_old" sheetId="5" r:id="rId6"/>
+    <sheet name="init_cond" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId8"/>
+    <sheet name="old_cond" sheetId="7" r:id="rId9"/>
+    <sheet name="Original_Prev" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="165">
   <si>
     <t>AGE-GROUP</t>
   </si>
@@ -542,7 +543,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -600,6 +601,13 @@
       <name val="Lucida Grande"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -628,7 +636,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -700,6 +708,17 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1372,6 +1391,158 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.5" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3">
+        <v>23.5</v>
+      </c>
+      <c r="C2" s="3">
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
+        <v>59.8</v>
+      </c>
+      <c r="C3" s="3">
+        <v>40.200000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3">
+        <v>82.7</v>
+      </c>
+      <c r="C4" s="3">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>91.4</v>
+      </c>
+      <c r="C5" s="3">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3">
+        <v>92.6</v>
+      </c>
+      <c r="C6" s="3">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3">
+        <v>92.9</v>
+      </c>
+      <c r="C7" s="3">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3">
+        <v>92.3</v>
+      </c>
+      <c r="C8" s="3">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4">
+        <v>91</v>
+      </c>
+      <c r="C9" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3">
+        <v>90.5</v>
+      </c>
+      <c r="C10" s="3">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3">
+        <v>90.8</v>
+      </c>
+      <c r="C11" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3">
+        <v>89.2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>10.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
@@ -7994,8 +8165,8 @@
   </sheetPr>
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11485,6 +11656,2897 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE56B1BC-D541-DB49-B52D-778AD4D27FD7}">
+  <dimension ref="A1:O64"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+    </row>
+    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="30">
+        <v>0</v>
+      </c>
+      <c r="B2" s="31">
+        <v>394858.96</v>
+      </c>
+      <c r="C2" s="30">
+        <v>60648</v>
+      </c>
+      <c r="D2" s="31">
+        <v>60648.27</v>
+      </c>
+      <c r="E2" s="30">
+        <v>0</v>
+      </c>
+      <c r="F2" s="31">
+        <v>516155.5</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="32">
+        <v>482465</v>
+      </c>
+      <c r="I2" s="32">
+        <v>476594</v>
+      </c>
+      <c r="J2" s="3">
+        <v>23.5</v>
+      </c>
+      <c r="K2" s="3">
+        <v>76.5</v>
+      </c>
+      <c r="L2" s="32">
+        <v>0</v>
+      </c>
+      <c r="M2" s="30">
+        <v>1</v>
+      </c>
+      <c r="N2" s="29"/>
+      <c r="O2" s="33" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="30">
+        <v>0</v>
+      </c>
+      <c r="B3" s="31">
+        <v>383511.33</v>
+      </c>
+      <c r="C3" s="30">
+        <v>58905</v>
+      </c>
+      <c r="D3" s="31">
+        <v>58905.34</v>
+      </c>
+      <c r="E3" s="30">
+        <v>0</v>
+      </c>
+      <c r="F3" s="30">
+        <v>501322</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="32">
+        <v>482465</v>
+      </c>
+      <c r="I3" s="32">
+        <v>476594</v>
+      </c>
+      <c r="J3" s="3">
+        <v>23.5</v>
+      </c>
+      <c r="K3" s="3">
+        <v>76.5</v>
+      </c>
+      <c r="L3" s="32">
+        <v>0</v>
+      </c>
+      <c r="M3" s="30">
+        <v>1</v>
+      </c>
+      <c r="N3" s="29"/>
+      <c r="O3" s="33" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="30">
+        <v>0</v>
+      </c>
+      <c r="B4" s="31">
+        <v>767022.66</v>
+      </c>
+      <c r="C4" s="30">
+        <v>117811</v>
+      </c>
+      <c r="D4" s="31">
+        <v>117810.67</v>
+      </c>
+      <c r="E4" s="30">
+        <v>0</v>
+      </c>
+      <c r="F4" s="32">
+        <v>1002644</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="32">
+        <v>462110</v>
+      </c>
+      <c r="I4" s="32">
+        <v>457041</v>
+      </c>
+      <c r="J4" s="3">
+        <v>23.5</v>
+      </c>
+      <c r="K4" s="3">
+        <v>76.5</v>
+      </c>
+      <c r="L4" s="32">
+        <v>0</v>
+      </c>
+      <c r="M4" s="30">
+        <v>1</v>
+      </c>
+      <c r="N4" s="29"/>
+      <c r="O4" s="33" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="30">
+        <v>0</v>
+      </c>
+      <c r="B5" s="31">
+        <v>745344.09</v>
+      </c>
+      <c r="C5" s="30">
+        <v>114481</v>
+      </c>
+      <c r="D5" s="31">
+        <v>114480.96000000001</v>
+      </c>
+      <c r="E5" s="30">
+        <v>0</v>
+      </c>
+      <c r="F5" s="32">
+        <v>974306</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="32">
+        <v>468475</v>
+      </c>
+      <c r="I5" s="32">
+        <v>462894</v>
+      </c>
+      <c r="J5" s="3">
+        <v>23.5</v>
+      </c>
+      <c r="K5" s="3">
+        <v>76.5</v>
+      </c>
+      <c r="L5" s="32">
+        <v>0</v>
+      </c>
+      <c r="M5" s="30">
+        <v>1</v>
+      </c>
+      <c r="N5" s="29"/>
+      <c r="O5" s="33" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="30">
+        <v>0</v>
+      </c>
+      <c r="B6" s="31">
+        <v>720550.44</v>
+      </c>
+      <c r="C6" s="30">
+        <v>110673</v>
+      </c>
+      <c r="D6" s="31">
+        <v>110672.78</v>
+      </c>
+      <c r="E6" s="30">
+        <v>0</v>
+      </c>
+      <c r="F6" s="32">
+        <v>941896</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="32">
+        <v>485954</v>
+      </c>
+      <c r="I6" s="32">
+        <v>480334</v>
+      </c>
+      <c r="J6" s="3">
+        <v>23.5</v>
+      </c>
+      <c r="K6" s="3">
+        <v>76.5</v>
+      </c>
+      <c r="L6" s="32">
+        <v>0</v>
+      </c>
+      <c r="M6" s="30">
+        <v>1</v>
+      </c>
+      <c r="N6" s="29"/>
+      <c r="O6" s="33" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="30">
+        <v>0</v>
+      </c>
+      <c r="B7" s="31">
+        <v>692695.26</v>
+      </c>
+      <c r="C7" s="30">
+        <v>106394</v>
+      </c>
+      <c r="D7" s="31">
+        <v>106394.37</v>
+      </c>
+      <c r="E7" s="30">
+        <v>0</v>
+      </c>
+      <c r="F7" s="32">
+        <v>905484</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="32">
+        <v>475715</v>
+      </c>
+      <c r="I7" s="32">
+        <v>471041</v>
+      </c>
+      <c r="J7" s="3">
+        <v>23.5</v>
+      </c>
+      <c r="K7" s="3">
+        <v>76.5</v>
+      </c>
+      <c r="L7" s="32">
+        <v>0</v>
+      </c>
+      <c r="M7" s="30">
+        <v>1</v>
+      </c>
+      <c r="N7" s="29"/>
+      <c r="O7" s="33" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="30">
+        <v>0</v>
+      </c>
+      <c r="B8" s="31">
+        <v>350178.98</v>
+      </c>
+      <c r="C8" s="30">
+        <v>130228</v>
+      </c>
+      <c r="D8" s="31">
+        <v>390684.76</v>
+      </c>
+      <c r="E8" s="30">
+        <v>0</v>
+      </c>
+      <c r="F8" s="32">
+        <v>871092</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="32">
+        <v>477195</v>
+      </c>
+      <c r="I8" s="32">
+        <v>474657</v>
+      </c>
+      <c r="J8" s="3">
+        <v>59.8</v>
+      </c>
+      <c r="K8" s="3">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="L8" s="32">
+        <v>0</v>
+      </c>
+      <c r="M8" s="30">
+        <v>1</v>
+      </c>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="30">
+        <v>0</v>
+      </c>
+      <c r="B9" s="31">
+        <v>338841.38</v>
+      </c>
+      <c r="C9" s="30">
+        <v>126012</v>
+      </c>
+      <c r="D9" s="31">
+        <v>378035.72</v>
+      </c>
+      <c r="E9" s="30">
+        <v>0</v>
+      </c>
+      <c r="F9" s="32">
+        <v>842889</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="32">
+        <v>477831</v>
+      </c>
+      <c r="I9" s="32">
+        <v>477149</v>
+      </c>
+      <c r="J9" s="3">
+        <v>59.8</v>
+      </c>
+      <c r="K9" s="3">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="L9" s="32">
+        <v>0</v>
+      </c>
+      <c r="M9" s="30">
+        <v>1</v>
+      </c>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="30">
+        <v>0</v>
+      </c>
+      <c r="B10" s="31">
+        <v>331579.25</v>
+      </c>
+      <c r="C10" s="30">
+        <v>123311</v>
+      </c>
+      <c r="D10" s="31">
+        <v>369933.56</v>
+      </c>
+      <c r="E10" s="30">
+        <v>0</v>
+      </c>
+      <c r="F10" s="32">
+        <v>824824</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="32">
+        <v>480036</v>
+      </c>
+      <c r="I10" s="32">
+        <v>480546</v>
+      </c>
+      <c r="J10" s="3">
+        <v>59.8</v>
+      </c>
+      <c r="K10" s="3">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="L10" s="32">
+        <v>0</v>
+      </c>
+      <c r="M10" s="30">
+        <v>1</v>
+      </c>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="30">
+        <v>0</v>
+      </c>
+      <c r="B11" s="31">
+        <v>327330.51</v>
+      </c>
+      <c r="C11" s="30">
+        <v>121731</v>
+      </c>
+      <c r="D11" s="31">
+        <v>365193.37</v>
+      </c>
+      <c r="E11" s="30">
+        <v>0</v>
+      </c>
+      <c r="F11" s="32">
+        <v>814255</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="32">
+        <v>482670</v>
+      </c>
+      <c r="I11" s="32">
+        <v>483803</v>
+      </c>
+      <c r="J11" s="3">
+        <v>59.8</v>
+      </c>
+      <c r="K11" s="3">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="L11" s="32">
+        <v>0</v>
+      </c>
+      <c r="M11" s="30">
+        <v>1</v>
+      </c>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="30">
+        <v>0</v>
+      </c>
+      <c r="B12" s="31">
+        <v>324290.99</v>
+      </c>
+      <c r="C12" s="30">
+        <v>120601</v>
+      </c>
+      <c r="D12" s="31">
+        <v>361802.26</v>
+      </c>
+      <c r="E12" s="30">
+        <v>0</v>
+      </c>
+      <c r="F12" s="32">
+        <v>806694</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="32">
+        <v>486005</v>
+      </c>
+      <c r="I12" s="32">
+        <v>487587</v>
+      </c>
+      <c r="J12" s="3">
+        <v>59.8</v>
+      </c>
+      <c r="K12" s="3">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="L12" s="32">
+        <v>0</v>
+      </c>
+      <c r="M12" s="30">
+        <v>1</v>
+      </c>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="30">
+        <v>0</v>
+      </c>
+      <c r="B13" s="31">
+        <v>137730.49</v>
+      </c>
+      <c r="C13" s="30">
+        <v>65840</v>
+      </c>
+      <c r="D13" s="31">
+        <v>592559.56000000006</v>
+      </c>
+      <c r="E13" s="30">
+        <v>0</v>
+      </c>
+      <c r="F13" s="32">
+        <v>796130</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="32">
+        <v>491006</v>
+      </c>
+      <c r="I13" s="32">
+        <v>492330</v>
+      </c>
+      <c r="J13" s="3">
+        <v>82.7</v>
+      </c>
+      <c r="K13" s="3">
+        <v>17.3</v>
+      </c>
+      <c r="L13" s="32">
+        <v>0</v>
+      </c>
+      <c r="M13" s="30">
+        <v>1</v>
+      </c>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="30">
+        <v>0</v>
+      </c>
+      <c r="B14" s="31">
+        <v>134983.42000000001</v>
+      </c>
+      <c r="C14" s="30">
+        <v>64527</v>
+      </c>
+      <c r="D14" s="31">
+        <v>580740.81999999995</v>
+      </c>
+      <c r="E14" s="30">
+        <v>0</v>
+      </c>
+      <c r="F14" s="32">
+        <v>780251</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="32">
+        <v>495010</v>
+      </c>
+      <c r="I14" s="32">
+        <v>496217</v>
+      </c>
+      <c r="J14" s="3">
+        <v>82.7</v>
+      </c>
+      <c r="K14" s="3">
+        <v>17.3</v>
+      </c>
+      <c r="L14" s="32">
+        <v>0</v>
+      </c>
+      <c r="M14" s="30">
+        <v>1</v>
+      </c>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="30">
+        <v>0</v>
+      </c>
+      <c r="B15" s="31">
+        <v>130949.93</v>
+      </c>
+      <c r="C15" s="30">
+        <v>62599</v>
+      </c>
+      <c r="D15" s="31">
+        <v>563387.46</v>
+      </c>
+      <c r="E15" s="30">
+        <v>0</v>
+      </c>
+      <c r="F15" s="32">
+        <v>756936</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" s="32">
+        <v>499272</v>
+      </c>
+      <c r="I15" s="32">
+        <v>501192</v>
+      </c>
+      <c r="J15" s="3">
+        <v>82.7</v>
+      </c>
+      <c r="K15" s="3">
+        <v>17.3</v>
+      </c>
+      <c r="L15" s="32">
+        <v>0</v>
+      </c>
+      <c r="M15" s="30">
+        <v>1</v>
+      </c>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="30">
+        <v>0</v>
+      </c>
+      <c r="B16" s="31">
+        <v>126140.18</v>
+      </c>
+      <c r="C16" s="30">
+        <v>60299</v>
+      </c>
+      <c r="D16" s="31">
+        <v>542694.43999999994</v>
+      </c>
+      <c r="E16" s="30">
+        <v>0</v>
+      </c>
+      <c r="F16" s="32">
+        <v>729134</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="32">
+        <v>502807</v>
+      </c>
+      <c r="I16" s="32">
+        <v>506168</v>
+      </c>
+      <c r="J16" s="3">
+        <v>82.7</v>
+      </c>
+      <c r="K16" s="3">
+        <v>17.3</v>
+      </c>
+      <c r="L16" s="32">
+        <v>0</v>
+      </c>
+      <c r="M16" s="30">
+        <v>1</v>
+      </c>
+      <c r="N16" s="29"/>
+      <c r="O16" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="30">
+        <v>0</v>
+      </c>
+      <c r="B17" s="31">
+        <v>121213.32</v>
+      </c>
+      <c r="C17" s="30">
+        <v>57944</v>
+      </c>
+      <c r="D17" s="31">
+        <v>521497.52</v>
+      </c>
+      <c r="E17" s="30">
+        <v>0</v>
+      </c>
+      <c r="F17" s="32">
+        <v>700655</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="32">
+        <v>506106</v>
+      </c>
+      <c r="I17" s="32">
+        <v>509191</v>
+      </c>
+      <c r="J17" s="3">
+        <v>82.7</v>
+      </c>
+      <c r="K17" s="3">
+        <v>17.3</v>
+      </c>
+      <c r="L17" s="32">
+        <v>0</v>
+      </c>
+      <c r="M17" s="30">
+        <v>1</v>
+      </c>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="30">
+        <v>0</v>
+      </c>
+      <c r="B18" s="31">
+        <v>58170.14</v>
+      </c>
+      <c r="C18" s="30">
+        <v>61823</v>
+      </c>
+      <c r="D18" s="31">
+        <v>556404.17000000004</v>
+      </c>
+      <c r="E18" s="30">
+        <v>0</v>
+      </c>
+      <c r="F18" s="32">
+        <v>676397</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="32">
+        <v>498707</v>
+      </c>
+      <c r="I18" s="32">
+        <v>503618</v>
+      </c>
+      <c r="J18" s="3">
+        <v>91.4</v>
+      </c>
+      <c r="K18" s="3">
+        <v>8.6</v>
+      </c>
+      <c r="L18" s="32">
+        <v>0</v>
+      </c>
+      <c r="M18" s="30">
+        <v>2</v>
+      </c>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="30">
+        <v>0</v>
+      </c>
+      <c r="B19" s="31">
+        <v>56660.5</v>
+      </c>
+      <c r="C19" s="30">
+        <v>60218</v>
+      </c>
+      <c r="D19" s="31">
+        <v>541964.25</v>
+      </c>
+      <c r="E19" s="30">
+        <v>0</v>
+      </c>
+      <c r="F19" s="32">
+        <v>658843</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="32">
+        <v>494286</v>
+      </c>
+      <c r="I19" s="32">
+        <v>500477</v>
+      </c>
+      <c r="J19" s="3">
+        <v>91.4</v>
+      </c>
+      <c r="K19" s="3">
+        <v>8.6</v>
+      </c>
+      <c r="L19" s="32">
+        <v>0</v>
+      </c>
+      <c r="M19" s="30">
+        <v>2</v>
+      </c>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="30">
+        <v>0</v>
+      </c>
+      <c r="B20" s="31">
+        <v>55902.49</v>
+      </c>
+      <c r="C20" s="30">
+        <v>59413</v>
+      </c>
+      <c r="D20" s="31">
+        <v>534713.86</v>
+      </c>
+      <c r="E20" s="30">
+        <v>0</v>
+      </c>
+      <c r="F20" s="32">
+        <v>650029</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="32">
+        <v>484387</v>
+      </c>
+      <c r="I20" s="32">
+        <v>491441</v>
+      </c>
+      <c r="J20" s="3">
+        <v>91.4</v>
+      </c>
+      <c r="K20" s="3">
+        <v>8.6</v>
+      </c>
+      <c r="L20" s="32">
+        <v>0</v>
+      </c>
+      <c r="M20" s="30">
+        <v>2</v>
+      </c>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="30">
+        <v>0</v>
+      </c>
+      <c r="B21" s="31">
+        <v>55638.559999999998</v>
+      </c>
+      <c r="C21" s="30">
+        <v>59132</v>
+      </c>
+      <c r="D21" s="31">
+        <v>532189.30000000005</v>
+      </c>
+      <c r="E21" s="30">
+        <v>0</v>
+      </c>
+      <c r="F21" s="32">
+        <v>646960</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" s="32">
+        <v>469743</v>
+      </c>
+      <c r="I21" s="32">
+        <v>477510</v>
+      </c>
+      <c r="J21" s="3">
+        <v>91.4</v>
+      </c>
+      <c r="K21" s="3">
+        <v>8.6</v>
+      </c>
+      <c r="L21" s="32">
+        <v>0</v>
+      </c>
+      <c r="M21" s="30">
+        <v>2</v>
+      </c>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="30">
+        <v>0</v>
+      </c>
+      <c r="B22" s="31">
+        <v>55485.65</v>
+      </c>
+      <c r="C22" s="30">
+        <v>58970</v>
+      </c>
+      <c r="D22" s="31">
+        <v>530726.71</v>
+      </c>
+      <c r="E22" s="30">
+        <v>0</v>
+      </c>
+      <c r="F22" s="32">
+        <v>645182</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H22" s="32">
+        <v>452511</v>
+      </c>
+      <c r="I22" s="32">
+        <v>461364</v>
+      </c>
+      <c r="J22" s="3">
+        <v>91.4</v>
+      </c>
+      <c r="K22" s="3">
+        <v>8.6</v>
+      </c>
+      <c r="L22" s="32">
+        <v>0</v>
+      </c>
+      <c r="M22" s="30">
+        <v>2</v>
+      </c>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="30">
+        <v>0</v>
+      </c>
+      <c r="B23" s="31">
+        <v>47427.86</v>
+      </c>
+      <c r="C23" s="30">
+        <v>59349</v>
+      </c>
+      <c r="D23" s="31">
+        <v>534140.23</v>
+      </c>
+      <c r="E23" s="30">
+        <v>0</v>
+      </c>
+      <c r="F23" s="32">
+        <v>640917</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="32">
+        <v>436116</v>
+      </c>
+      <c r="I23" s="32">
+        <v>446657</v>
+      </c>
+      <c r="J23" s="3">
+        <v>92.6</v>
+      </c>
+      <c r="K23" s="3">
+        <v>7.4</v>
+      </c>
+      <c r="L23" s="32">
+        <v>0</v>
+      </c>
+      <c r="M23" s="30">
+        <v>3</v>
+      </c>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="30">
+        <v>0</v>
+      </c>
+      <c r="B24" s="31">
+        <v>46890.99</v>
+      </c>
+      <c r="C24" s="30">
+        <v>58677</v>
+      </c>
+      <c r="D24" s="31">
+        <v>528093.91</v>
+      </c>
+      <c r="E24" s="30">
+        <v>0</v>
+      </c>
+      <c r="F24" s="32">
+        <v>633662</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="32">
+        <v>422640</v>
+      </c>
+      <c r="I24" s="32">
+        <v>435420</v>
+      </c>
+      <c r="J24" s="3">
+        <v>92.6</v>
+      </c>
+      <c r="K24" s="3">
+        <v>7.4</v>
+      </c>
+      <c r="L24" s="32">
+        <v>0</v>
+      </c>
+      <c r="M24" s="30">
+        <v>3</v>
+      </c>
+      <c r="N24" s="29"/>
+      <c r="O24" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="30">
+        <v>0</v>
+      </c>
+      <c r="B25" s="31">
+        <v>46002.69</v>
+      </c>
+      <c r="C25" s="30">
+        <v>57566</v>
+      </c>
+      <c r="D25" s="31">
+        <v>518089.78</v>
+      </c>
+      <c r="E25" s="30">
+        <v>0</v>
+      </c>
+      <c r="F25" s="32">
+        <v>621658</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H25" s="32">
+        <v>414150</v>
+      </c>
+      <c r="I25" s="32">
+        <v>429344</v>
+      </c>
+      <c r="J25" s="3">
+        <v>92.6</v>
+      </c>
+      <c r="K25" s="3">
+        <v>7.4</v>
+      </c>
+      <c r="L25" s="32">
+        <v>0</v>
+      </c>
+      <c r="M25" s="30">
+        <v>3</v>
+      </c>
+      <c r="N25" s="29"/>
+      <c r="O25" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="30">
+        <v>0</v>
+      </c>
+      <c r="B26" s="31">
+        <v>44830.98</v>
+      </c>
+      <c r="C26" s="30">
+        <v>56099</v>
+      </c>
+      <c r="D26" s="31">
+        <v>504893.72</v>
+      </c>
+      <c r="E26" s="30">
+        <v>0</v>
+      </c>
+      <c r="F26" s="32">
+        <v>605824</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="32">
+        <v>409384</v>
+      </c>
+      <c r="I26" s="32">
+        <v>426907</v>
+      </c>
+      <c r="J26" s="3">
+        <v>92.6</v>
+      </c>
+      <c r="K26" s="3">
+        <v>7.4</v>
+      </c>
+      <c r="L26" s="32">
+        <v>0</v>
+      </c>
+      <c r="M26" s="30">
+        <v>3</v>
+      </c>
+      <c r="N26" s="29"/>
+      <c r="O26" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="30">
+        <v>0</v>
+      </c>
+      <c r="B27" s="31">
+        <v>43581.49</v>
+      </c>
+      <c r="C27" s="30">
+        <v>54536</v>
+      </c>
+      <c r="D27" s="31">
+        <v>490821.76</v>
+      </c>
+      <c r="E27" s="30">
+        <v>0</v>
+      </c>
+      <c r="F27" s="32">
+        <v>588939</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="32">
+        <v>405844</v>
+      </c>
+      <c r="I27" s="32">
+        <v>425445</v>
+      </c>
+      <c r="J27" s="3">
+        <v>92.6</v>
+      </c>
+      <c r="K27" s="3">
+        <v>7.4</v>
+      </c>
+      <c r="L27" s="32">
+        <v>0</v>
+      </c>
+      <c r="M27" s="30">
+        <v>3</v>
+      </c>
+      <c r="N27" s="29"/>
+      <c r="O27" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="30">
+        <v>0</v>
+      </c>
+      <c r="B28" s="31">
+        <v>40618.6</v>
+      </c>
+      <c r="C28" s="30">
+        <v>53147</v>
+      </c>
+      <c r="D28" s="31">
+        <v>478326.96</v>
+      </c>
+      <c r="E28" s="30">
+        <v>0</v>
+      </c>
+      <c r="F28" s="32">
+        <v>572093</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H28" s="32">
+        <v>400498</v>
+      </c>
+      <c r="I28" s="32">
+        <v>421856</v>
+      </c>
+      <c r="J28" s="3">
+        <v>92.9</v>
+      </c>
+      <c r="K28" s="3">
+        <v>7.1</v>
+      </c>
+      <c r="L28" s="32">
+        <v>0</v>
+      </c>
+      <c r="M28" s="30">
+        <v>4</v>
+      </c>
+      <c r="N28" s="29"/>
+      <c r="O28" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="30">
+        <v>0</v>
+      </c>
+      <c r="B29" s="31">
+        <v>39321.58</v>
+      </c>
+      <c r="C29" s="30">
+        <v>51450</v>
+      </c>
+      <c r="D29" s="31">
+        <v>463053.08</v>
+      </c>
+      <c r="E29" s="30">
+        <v>0</v>
+      </c>
+      <c r="F29" s="32">
+        <v>553825</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H29" s="32">
+        <v>392439</v>
+      </c>
+      <c r="I29" s="32">
+        <v>415011</v>
+      </c>
+      <c r="J29" s="3">
+        <v>92.9</v>
+      </c>
+      <c r="K29" s="3">
+        <v>7.1</v>
+      </c>
+      <c r="L29" s="32">
+        <v>0</v>
+      </c>
+      <c r="M29" s="30">
+        <v>4</v>
+      </c>
+      <c r="N29" s="29"/>
+      <c r="O29" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="30">
+        <v>0</v>
+      </c>
+      <c r="B30" s="31">
+        <v>37940.839999999997</v>
+      </c>
+      <c r="C30" s="30">
+        <v>49644</v>
+      </c>
+      <c r="D30" s="31">
+        <v>446793.45</v>
+      </c>
+      <c r="E30" s="30">
+        <v>0</v>
+      </c>
+      <c r="F30" s="32">
+        <v>534378</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="H30" s="32">
+        <v>380565</v>
+      </c>
+      <c r="I30" s="32">
+        <v>403968</v>
+      </c>
+      <c r="J30" s="3">
+        <v>92.9</v>
+      </c>
+      <c r="K30" s="3">
+        <v>7.1</v>
+      </c>
+      <c r="L30" s="32">
+        <v>0</v>
+      </c>
+      <c r="M30" s="30">
+        <v>4</v>
+      </c>
+      <c r="N30" s="29"/>
+      <c r="O30" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="30">
+        <v>0</v>
+      </c>
+      <c r="B31" s="31">
+        <v>36512.82</v>
+      </c>
+      <c r="C31" s="30">
+        <v>47775</v>
+      </c>
+      <c r="D31" s="31">
+        <v>429976.97</v>
+      </c>
+      <c r="E31" s="30">
+        <v>0</v>
+      </c>
+      <c r="F31" s="32">
+        <v>514265</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H31" s="32">
+        <v>366136</v>
+      </c>
+      <c r="I31" s="32">
+        <v>390065</v>
+      </c>
+      <c r="J31" s="3">
+        <v>92.9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>7.1</v>
+      </c>
+      <c r="L31" s="32">
+        <v>0</v>
+      </c>
+      <c r="M31" s="30">
+        <v>4</v>
+      </c>
+      <c r="N31" s="29"/>
+      <c r="O31" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="30">
+        <v>0</v>
+      </c>
+      <c r="B32" s="31">
+        <v>35054.26</v>
+      </c>
+      <c r="C32" s="30">
+        <v>45867</v>
+      </c>
+      <c r="D32" s="31">
+        <v>412800.96</v>
+      </c>
+      <c r="E32" s="30">
+        <v>0</v>
+      </c>
+      <c r="F32" s="32">
+        <v>493722</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H32" s="32">
+        <v>351004</v>
+      </c>
+      <c r="I32" s="32">
+        <v>375193</v>
+      </c>
+      <c r="J32" s="3">
+        <v>92.9</v>
+      </c>
+      <c r="K32" s="3">
+        <v>7.1</v>
+      </c>
+      <c r="L32" s="32">
+        <v>0</v>
+      </c>
+      <c r="M32" s="30">
+        <v>4</v>
+      </c>
+      <c r="N32" s="29"/>
+      <c r="O32" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="30">
+        <v>0</v>
+      </c>
+      <c r="B33" s="31">
+        <v>36446.800000000003</v>
+      </c>
+      <c r="C33" s="30">
+        <v>43689</v>
+      </c>
+      <c r="D33" s="31">
+        <v>393199.38</v>
+      </c>
+      <c r="E33" s="30">
+        <v>0</v>
+      </c>
+      <c r="F33" s="32">
+        <v>473335</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="H33" s="32">
+        <v>337393</v>
+      </c>
+      <c r="I33" s="32">
+        <v>361956</v>
+      </c>
+      <c r="J33" s="3">
+        <v>92.3</v>
+      </c>
+      <c r="K33" s="3">
+        <v>7.7</v>
+      </c>
+      <c r="L33" s="32">
+        <v>0</v>
+      </c>
+      <c r="M33" s="30">
+        <v>5</v>
+      </c>
+      <c r="N33" s="29"/>
+      <c r="O33" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="30">
+        <v>0</v>
+      </c>
+      <c r="B34" s="31">
+        <v>34937.599999999999</v>
+      </c>
+      <c r="C34" s="30">
+        <v>41880</v>
+      </c>
+      <c r="D34" s="31">
+        <v>376917.66</v>
+      </c>
+      <c r="E34" s="30">
+        <v>0</v>
+      </c>
+      <c r="F34" s="32">
+        <v>453735</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="H34" s="32">
+        <v>326161</v>
+      </c>
+      <c r="I34" s="32">
+        <v>351775</v>
+      </c>
+      <c r="J34" s="3">
+        <v>92.3</v>
+      </c>
+      <c r="K34" s="3">
+        <v>7.7</v>
+      </c>
+      <c r="L34" s="32">
+        <v>0</v>
+      </c>
+      <c r="M34" s="30">
+        <v>5</v>
+      </c>
+      <c r="N34" s="29"/>
+      <c r="O34" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="30">
+        <v>0</v>
+      </c>
+      <c r="B35" s="31">
+        <v>33516.410000000003</v>
+      </c>
+      <c r="C35" s="30">
+        <v>40176</v>
+      </c>
+      <c r="D35" s="31">
+        <v>361585.43</v>
+      </c>
+      <c r="E35" s="30">
+        <v>0</v>
+      </c>
+      <c r="F35" s="32">
+        <v>435278</v>
+      </c>
+      <c r="G35" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H35" s="32">
+        <v>318277</v>
+      </c>
+      <c r="I35" s="32">
+        <v>345598</v>
+      </c>
+      <c r="J35" s="3">
+        <v>92.3</v>
+      </c>
+      <c r="K35" s="3">
+        <v>7.7</v>
+      </c>
+      <c r="L35" s="32">
+        <v>0</v>
+      </c>
+      <c r="M35" s="30">
+        <v>5</v>
+      </c>
+      <c r="N35" s="29"/>
+      <c r="O35" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="30">
+        <v>0</v>
+      </c>
+      <c r="B36" s="31">
+        <v>32160.59</v>
+      </c>
+      <c r="C36" s="30">
+        <v>38551</v>
+      </c>
+      <c r="D36" s="31">
+        <v>346958.47</v>
+      </c>
+      <c r="E36" s="30">
+        <v>0</v>
+      </c>
+      <c r="F36" s="32">
+        <v>417670</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H36" s="32">
+        <v>312710</v>
+      </c>
+      <c r="I36" s="32">
+        <v>342036</v>
+      </c>
+      <c r="J36" s="3">
+        <v>92.3</v>
+      </c>
+      <c r="K36" s="3">
+        <v>7.7</v>
+      </c>
+      <c r="L36" s="32">
+        <v>0</v>
+      </c>
+      <c r="M36" s="30">
+        <v>5</v>
+      </c>
+      <c r="N36" s="29"/>
+      <c r="O36" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="30">
+        <v>0</v>
+      </c>
+      <c r="B37" s="31">
+        <v>30865.14</v>
+      </c>
+      <c r="C37" s="30">
+        <v>36998</v>
+      </c>
+      <c r="D37" s="31">
+        <v>332982.77</v>
+      </c>
+      <c r="E37" s="30">
+        <v>0</v>
+      </c>
+      <c r="F37" s="32">
+        <v>400846</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H37" s="32">
+        <v>307842</v>
+      </c>
+      <c r="I37" s="32">
+        <v>339157</v>
+      </c>
+      <c r="J37" s="3">
+        <v>92.3</v>
+      </c>
+      <c r="K37" s="3">
+        <v>7.7</v>
+      </c>
+      <c r="L37" s="32">
+        <v>0</v>
+      </c>
+      <c r="M37" s="30">
+        <v>5</v>
+      </c>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="30">
+        <v>0</v>
+      </c>
+      <c r="B38" s="31">
+        <v>34563.599999999999</v>
+      </c>
+      <c r="C38" s="30">
+        <v>34948</v>
+      </c>
+      <c r="D38" s="31">
+        <v>314528.76</v>
+      </c>
+      <c r="E38" s="30">
+        <v>0</v>
+      </c>
+      <c r="F38" s="32">
+        <v>384040</v>
+      </c>
+      <c r="G38" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="H38" s="32">
+        <v>302373</v>
+      </c>
+      <c r="I38" s="32">
+        <v>334992</v>
+      </c>
+      <c r="J38" s="4">
+        <v>91</v>
+      </c>
+      <c r="K38" s="4">
+        <v>9</v>
+      </c>
+      <c r="L38" s="32">
+        <v>0</v>
+      </c>
+      <c r="M38" s="30">
+        <v>6</v>
+      </c>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="30">
+        <v>0</v>
+      </c>
+      <c r="B39" s="31">
+        <v>32984.639999999999</v>
+      </c>
+      <c r="C39" s="30">
+        <v>33351</v>
+      </c>
+      <c r="D39" s="31">
+        <v>300160.21999999997</v>
+      </c>
+      <c r="E39" s="30">
+        <v>0</v>
+      </c>
+      <c r="F39" s="32">
+        <v>366496</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H39" s="32">
+        <v>296389</v>
+      </c>
+      <c r="I39" s="32">
+        <v>329032</v>
+      </c>
+      <c r="J39" s="4">
+        <v>91</v>
+      </c>
+      <c r="K39" s="4">
+        <v>9</v>
+      </c>
+      <c r="L39" s="32">
+        <v>0</v>
+      </c>
+      <c r="M39" s="30">
+        <v>6</v>
+      </c>
+      <c r="N39" s="29"/>
+      <c r="O39" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="30">
+        <v>0</v>
+      </c>
+      <c r="B40" s="31">
+        <v>31308.3</v>
+      </c>
+      <c r="C40" s="30">
+        <v>31656</v>
+      </c>
+      <c r="D40" s="31">
+        <v>284905.53000000003</v>
+      </c>
+      <c r="E40" s="30">
+        <v>0</v>
+      </c>
+      <c r="F40" s="32">
+        <v>347870</v>
+      </c>
+      <c r="G40" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="H40" s="32">
+        <v>289132</v>
+      </c>
+      <c r="I40" s="32">
+        <v>320429</v>
+      </c>
+      <c r="J40" s="4">
+        <v>91</v>
+      </c>
+      <c r="K40" s="4">
+        <v>9</v>
+      </c>
+      <c r="L40" s="32">
+        <v>0</v>
+      </c>
+      <c r="M40" s="30">
+        <v>6</v>
+      </c>
+      <c r="N40" s="29"/>
+      <c r="O40" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="30">
+        <v>0</v>
+      </c>
+      <c r="B41" s="31">
+        <v>29610.720000000001</v>
+      </c>
+      <c r="C41" s="30">
+        <v>29940</v>
+      </c>
+      <c r="D41" s="31">
+        <v>269457.55</v>
+      </c>
+      <c r="E41" s="30">
+        <v>0</v>
+      </c>
+      <c r="F41" s="32">
+        <v>329008</v>
+      </c>
+      <c r="G41" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="H41" s="32">
+        <v>280740</v>
+      </c>
+      <c r="I41" s="32">
+        <v>309860</v>
+      </c>
+      <c r="J41" s="4">
+        <v>91</v>
+      </c>
+      <c r="K41" s="4">
+        <v>9</v>
+      </c>
+      <c r="L41" s="32">
+        <v>0</v>
+      </c>
+      <c r="M41" s="30">
+        <v>6</v>
+      </c>
+      <c r="N41" s="29"/>
+      <c r="O41" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="30">
+        <v>0</v>
+      </c>
+      <c r="B42" s="31">
+        <v>27876.87</v>
+      </c>
+      <c r="C42" s="30">
+        <v>28187</v>
+      </c>
+      <c r="D42" s="31">
+        <v>253679.52</v>
+      </c>
+      <c r="E42" s="30">
+        <v>0</v>
+      </c>
+      <c r="F42" s="32">
+        <v>309743</v>
+      </c>
+      <c r="G42" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H42" s="32">
+        <v>272042</v>
+      </c>
+      <c r="I42" s="32">
+        <v>298807</v>
+      </c>
+      <c r="J42" s="4">
+        <v>91</v>
+      </c>
+      <c r="K42" s="4">
+        <v>9</v>
+      </c>
+      <c r="L42" s="32">
+        <v>0</v>
+      </c>
+      <c r="M42" s="30">
+        <v>6</v>
+      </c>
+      <c r="N42" s="29"/>
+      <c r="O42" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="30">
+        <v>0</v>
+      </c>
+      <c r="B43" s="31">
+        <v>27774.3</v>
+      </c>
+      <c r="C43" s="30">
+        <v>26459</v>
+      </c>
+      <c r="D43" s="31">
+        <v>238128.03</v>
+      </c>
+      <c r="E43" s="30">
+        <v>0</v>
+      </c>
+      <c r="F43" s="32">
+        <v>292361</v>
+      </c>
+      <c r="G43" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H43" s="32">
+        <v>263140</v>
+      </c>
+      <c r="I43" s="32">
+        <v>288069</v>
+      </c>
+      <c r="J43" s="3">
+        <v>90.5</v>
+      </c>
+      <c r="K43" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="L43" s="32">
+        <v>0</v>
+      </c>
+      <c r="M43" s="30">
+        <v>7</v>
+      </c>
+      <c r="N43" s="29"/>
+      <c r="O43" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="30">
+        <v>0</v>
+      </c>
+      <c r="B44" s="31">
+        <v>26588.79</v>
+      </c>
+      <c r="C44" s="30">
+        <v>25329</v>
+      </c>
+      <c r="D44" s="31">
+        <v>227963.89</v>
+      </c>
+      <c r="E44" s="30">
+        <v>0</v>
+      </c>
+      <c r="F44" s="32">
+        <v>279882</v>
+      </c>
+      <c r="G44" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H44" s="32">
+        <v>253246</v>
+      </c>
+      <c r="I44" s="32">
+        <v>277133</v>
+      </c>
+      <c r="J44" s="3">
+        <v>90.5</v>
+      </c>
+      <c r="K44" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="L44" s="32">
+        <v>0</v>
+      </c>
+      <c r="M44" s="30">
+        <v>7</v>
+      </c>
+      <c r="N44" s="29"/>
+      <c r="O44" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="30">
+        <v>0</v>
+      </c>
+      <c r="B45" s="31">
+        <v>26024.02</v>
+      </c>
+      <c r="C45" s="30">
+        <v>24791</v>
+      </c>
+      <c r="D45" s="31">
+        <v>223121.69</v>
+      </c>
+      <c r="E45" s="30">
+        <v>0</v>
+      </c>
+      <c r="F45" s="32">
+        <v>273937</v>
+      </c>
+      <c r="G45" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H45" s="32">
+        <v>242433</v>
+      </c>
+      <c r="I45" s="32">
+        <v>266222</v>
+      </c>
+      <c r="J45" s="3">
+        <v>90.5</v>
+      </c>
+      <c r="K45" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="L45" s="32">
+        <v>0</v>
+      </c>
+      <c r="M45" s="30">
+        <v>7</v>
+      </c>
+      <c r="N45" s="29"/>
+      <c r="O45" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="30">
+        <v>0</v>
+      </c>
+      <c r="B46" s="31">
+        <v>25914.77</v>
+      </c>
+      <c r="C46" s="30">
+        <v>24687</v>
+      </c>
+      <c r="D46" s="31">
+        <v>222185.01</v>
+      </c>
+      <c r="E46" s="30">
+        <v>0</v>
+      </c>
+      <c r="F46" s="32">
+        <v>272787</v>
+      </c>
+      <c r="G46" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="H46" s="32">
+        <v>231089</v>
+      </c>
+      <c r="I46" s="32">
+        <v>255355</v>
+      </c>
+      <c r="J46" s="3">
+        <v>90.5</v>
+      </c>
+      <c r="K46" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="L46" s="32">
+        <v>0</v>
+      </c>
+      <c r="M46" s="30">
+        <v>7</v>
+      </c>
+      <c r="N46" s="29"/>
+      <c r="O46" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="30">
+        <v>0</v>
+      </c>
+      <c r="B47" s="31">
+        <v>26038.080000000002</v>
+      </c>
+      <c r="C47" s="30">
+        <v>24805</v>
+      </c>
+      <c r="D47" s="31">
+        <v>223242.23</v>
+      </c>
+      <c r="E47" s="30">
+        <v>0</v>
+      </c>
+      <c r="F47" s="32">
+        <v>274085</v>
+      </c>
+      <c r="G47" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="H47" s="32">
+        <v>219561</v>
+      </c>
+      <c r="I47" s="32">
+        <v>244397</v>
+      </c>
+      <c r="J47" s="3">
+        <v>90.5</v>
+      </c>
+      <c r="K47" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="L47" s="32">
+        <v>0</v>
+      </c>
+      <c r="M47" s="30">
+        <v>7</v>
+      </c>
+      <c r="N47" s="29"/>
+      <c r="O47" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="30">
+        <v>0</v>
+      </c>
+      <c r="B48" s="31">
+        <v>25247.93</v>
+      </c>
+      <c r="C48" s="30">
+        <v>24919</v>
+      </c>
+      <c r="D48" s="31">
+        <v>224267.46</v>
+      </c>
+      <c r="E48" s="30">
+        <v>0</v>
+      </c>
+      <c r="F48" s="32">
+        <v>274434</v>
+      </c>
+      <c r="G48" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H48" s="32">
+        <v>208392</v>
+      </c>
+      <c r="I48" s="32">
+        <v>233379</v>
+      </c>
+      <c r="J48" s="3">
+        <v>90.8</v>
+      </c>
+      <c r="K48" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L48" s="32">
+        <v>0</v>
+      </c>
+      <c r="M48" s="30">
+        <v>8</v>
+      </c>
+      <c r="N48" s="29"/>
+      <c r="O48" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="30">
+        <v>0</v>
+      </c>
+      <c r="B49" s="31">
+        <v>25017.01</v>
+      </c>
+      <c r="C49" s="30">
+        <v>24691</v>
+      </c>
+      <c r="D49" s="31">
+        <v>222216.29</v>
+      </c>
+      <c r="E49" s="30">
+        <v>0</v>
+      </c>
+      <c r="F49" s="32">
+        <v>271924</v>
+      </c>
+      <c r="G49" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H49" s="32">
+        <v>197996</v>
+      </c>
+      <c r="I49" s="32">
+        <v>222529</v>
+      </c>
+      <c r="J49" s="3">
+        <v>90.8</v>
+      </c>
+      <c r="K49" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L49" s="32">
+        <v>0</v>
+      </c>
+      <c r="M49" s="30">
+        <v>8</v>
+      </c>
+      <c r="N49" s="29"/>
+      <c r="O49" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="30">
+        <v>0</v>
+      </c>
+      <c r="B50" s="31">
+        <v>24339.89</v>
+      </c>
+      <c r="C50" s="30">
+        <v>24022</v>
+      </c>
+      <c r="D50" s="31">
+        <v>216201.7</v>
+      </c>
+      <c r="E50" s="30">
+        <v>0</v>
+      </c>
+      <c r="F50" s="32">
+        <v>264564</v>
+      </c>
+      <c r="G50" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="H50" s="32">
+        <v>188618</v>
+      </c>
+      <c r="I50" s="32">
+        <v>211955</v>
+      </c>
+      <c r="J50" s="3">
+        <v>90.8</v>
+      </c>
+      <c r="K50" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L50" s="32">
+        <v>0</v>
+      </c>
+      <c r="M50" s="30">
+        <v>8</v>
+      </c>
+      <c r="N50" s="29"/>
+      <c r="O50" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="30">
+        <v>0</v>
+      </c>
+      <c r="B51" s="31">
+        <v>23329.54</v>
+      </c>
+      <c r="C51" s="30">
+        <v>23025</v>
+      </c>
+      <c r="D51" s="31">
+        <v>207227.21</v>
+      </c>
+      <c r="E51" s="30">
+        <v>0</v>
+      </c>
+      <c r="F51" s="32">
+        <v>253582</v>
+      </c>
+      <c r="G51" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="H51" s="32">
+        <v>179999</v>
+      </c>
+      <c r="I51" s="32">
+        <v>201680</v>
+      </c>
+      <c r="J51" s="3">
+        <v>90.8</v>
+      </c>
+      <c r="K51" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L51" s="32">
+        <v>0</v>
+      </c>
+      <c r="M51" s="30">
+        <v>8</v>
+      </c>
+      <c r="N51" s="29"/>
+      <c r="O51" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="30">
+        <v>0</v>
+      </c>
+      <c r="B52" s="31">
+        <v>22225.91</v>
+      </c>
+      <c r="C52" s="30">
+        <v>21936</v>
+      </c>
+      <c r="D52" s="31">
+        <v>197424.08</v>
+      </c>
+      <c r="E52" s="30">
+        <v>0</v>
+      </c>
+      <c r="F52" s="32">
+        <v>241586</v>
+      </c>
+      <c r="G52" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="H52" s="32">
+        <v>171875</v>
+      </c>
+      <c r="I52" s="32">
+        <v>191894</v>
+      </c>
+      <c r="J52" s="3">
+        <v>90.8</v>
+      </c>
+      <c r="K52" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L52" s="32">
+        <v>0</v>
+      </c>
+      <c r="M52" s="30">
+        <v>8</v>
+      </c>
+      <c r="N52" s="29"/>
+      <c r="O52" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="30">
+        <v>0</v>
+      </c>
+      <c r="B53" s="31">
+        <v>24933.96</v>
+      </c>
+      <c r="C53" s="30">
+        <v>20594</v>
+      </c>
+      <c r="D53" s="31">
+        <v>185342.44</v>
+      </c>
+      <c r="E53" s="30">
+        <v>0</v>
+      </c>
+      <c r="F53" s="32">
+        <v>230870</v>
+      </c>
+      <c r="G53" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="H53" s="32">
+        <v>163684</v>
+      </c>
+      <c r="I53" s="32">
+        <v>182391</v>
+      </c>
+      <c r="J53" s="3">
+        <v>89.2</v>
+      </c>
+      <c r="K53" s="3">
+        <v>10.8</v>
+      </c>
+      <c r="L53" s="32">
+        <v>0</v>
+      </c>
+      <c r="M53" s="30">
+        <v>9</v>
+      </c>
+      <c r="N53" s="29"/>
+      <c r="O53" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="30">
+        <v>0</v>
+      </c>
+      <c r="B54" s="31">
+        <v>23952.240000000002</v>
+      </c>
+      <c r="C54" s="30">
+        <v>19783</v>
+      </c>
+      <c r="D54" s="31">
+        <v>178044.98</v>
+      </c>
+      <c r="E54" s="30">
+        <v>0</v>
+      </c>
+      <c r="F54" s="32">
+        <v>221780</v>
+      </c>
+      <c r="G54" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H54" s="32">
+        <v>155019</v>
+      </c>
+      <c r="I54" s="32">
+        <v>172819</v>
+      </c>
+      <c r="J54" s="3">
+        <v>89.2</v>
+      </c>
+      <c r="K54" s="3">
+        <v>10.8</v>
+      </c>
+      <c r="L54" s="32">
+        <v>0</v>
+      </c>
+      <c r="M54" s="30">
+        <v>9</v>
+      </c>
+      <c r="N54" s="29"/>
+      <c r="O54" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="30">
+        <v>0</v>
+      </c>
+      <c r="B55" s="31">
+        <v>23242.68</v>
+      </c>
+      <c r="C55" s="30">
+        <v>19197</v>
+      </c>
+      <c r="D55" s="31">
+        <v>172770.59</v>
+      </c>
+      <c r="E55" s="30">
+        <v>0</v>
+      </c>
+      <c r="F55" s="32">
+        <v>215210</v>
+      </c>
+      <c r="G55" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H55" s="32">
+        <v>145635</v>
+      </c>
+      <c r="I55" s="32">
+        <v>163038</v>
+      </c>
+      <c r="J55" s="3">
+        <v>89.2</v>
+      </c>
+      <c r="K55" s="3">
+        <v>10.8</v>
+      </c>
+      <c r="L55" s="32">
+        <v>0</v>
+      </c>
+      <c r="M55" s="30">
+        <v>9</v>
+      </c>
+      <c r="N55" s="29"/>
+      <c r="O55" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="30">
+        <v>0</v>
+      </c>
+      <c r="B56" s="31">
+        <v>22735.94</v>
+      </c>
+      <c r="C56" s="30">
+        <v>18778</v>
+      </c>
+      <c r="D56" s="31">
+        <v>169003.85</v>
+      </c>
+      <c r="E56" s="30">
+        <v>0</v>
+      </c>
+      <c r="F56" s="32">
+        <v>210518</v>
+      </c>
+      <c r="G56" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H56" s="32">
+        <v>135921</v>
+      </c>
+      <c r="I56" s="32">
+        <v>153353</v>
+      </c>
+      <c r="J56" s="3">
+        <v>89.2</v>
+      </c>
+      <c r="K56" s="3">
+        <v>10.8</v>
+      </c>
+      <c r="L56" s="32">
+        <v>0</v>
+      </c>
+      <c r="M56" s="30">
+        <v>9</v>
+      </c>
+      <c r="N56" s="29"/>
+      <c r="O56" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="30">
+        <v>0</v>
+      </c>
+      <c r="B57" s="31">
+        <v>22336.78</v>
+      </c>
+      <c r="C57" s="30">
+        <v>18449</v>
+      </c>
+      <c r="D57" s="31">
+        <v>166036.70000000001</v>
+      </c>
+      <c r="E57" s="30">
+        <v>0</v>
+      </c>
+      <c r="F57" s="32">
+        <v>206822</v>
+      </c>
+      <c r="G57" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H57" s="32">
+        <v>126022</v>
+      </c>
+      <c r="I57" s="32">
+        <v>143480</v>
+      </c>
+      <c r="J57" s="3">
+        <v>89.2</v>
+      </c>
+      <c r="K57" s="3">
+        <v>10.8</v>
+      </c>
+      <c r="L57" s="32">
+        <v>0</v>
+      </c>
+      <c r="M57" s="30">
+        <v>9</v>
+      </c>
+      <c r="N57" s="29"/>
+      <c r="O57" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="30">
+        <v>0</v>
+      </c>
+      <c r="B58" s="31">
+        <v>21859.52</v>
+      </c>
+      <c r="C58" s="30">
+        <v>18054</v>
+      </c>
+      <c r="D58" s="31">
+        <v>162489.13</v>
+      </c>
+      <c r="E58" s="30">
+        <v>0</v>
+      </c>
+      <c r="F58" s="32">
+        <v>202403</v>
+      </c>
+      <c r="G58" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="H58" s="32">
+        <v>116903</v>
+      </c>
+      <c r="I58" s="32">
+        <v>134499</v>
+      </c>
+      <c r="J58" s="3">
+        <v>89.2</v>
+      </c>
+      <c r="K58" s="3">
+        <v>10.8</v>
+      </c>
+      <c r="L58" s="32">
+        <v>0</v>
+      </c>
+      <c r="M58" s="30">
+        <v>10</v>
+      </c>
+      <c r="N58" s="29"/>
+      <c r="O58" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="30">
+        <v>0</v>
+      </c>
+      <c r="B59" s="31">
+        <v>21178.15</v>
+      </c>
+      <c r="C59" s="30">
+        <v>17492</v>
+      </c>
+      <c r="D59" s="31">
+        <v>157424.26</v>
+      </c>
+      <c r="E59" s="30">
+        <v>0</v>
+      </c>
+      <c r="F59" s="32">
+        <v>196094</v>
+      </c>
+      <c r="G59" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="H59" s="32">
+        <v>109625</v>
+      </c>
+      <c r="I59" s="32">
+        <v>127989</v>
+      </c>
+      <c r="J59" s="3">
+        <v>89.2</v>
+      </c>
+      <c r="K59" s="3">
+        <v>10.8</v>
+      </c>
+      <c r="L59" s="32">
+        <v>0</v>
+      </c>
+      <c r="M59" s="30">
+        <v>10</v>
+      </c>
+      <c r="N59" s="29"/>
+      <c r="O59" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="30">
+        <v>0</v>
+      </c>
+      <c r="B60" s="31">
+        <v>20165.759999999998</v>
+      </c>
+      <c r="C60" s="30">
+        <v>16655</v>
+      </c>
+      <c r="D60" s="31">
+        <v>149898.82</v>
+      </c>
+      <c r="E60" s="30">
+        <v>0</v>
+      </c>
+      <c r="F60" s="32">
+        <v>186720</v>
+      </c>
+      <c r="G60" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H60" s="32">
+        <v>104767</v>
+      </c>
+      <c r="I60" s="32">
+        <v>124746</v>
+      </c>
+      <c r="J60" s="3">
+        <v>89.2</v>
+      </c>
+      <c r="K60" s="3">
+        <v>10.8</v>
+      </c>
+      <c r="L60" s="32">
+        <v>0</v>
+      </c>
+      <c r="M60" s="30">
+        <v>10</v>
+      </c>
+      <c r="N60" s="29"/>
+      <c r="O60" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="30">
+        <v>0</v>
+      </c>
+      <c r="B61" s="31">
+        <v>18899.68</v>
+      </c>
+      <c r="C61" s="30">
+        <v>15610</v>
+      </c>
+      <c r="D61" s="31">
+        <v>140487.59</v>
+      </c>
+      <c r="E61" s="30">
+        <v>0</v>
+      </c>
+      <c r="F61" s="32">
+        <v>174997</v>
+      </c>
+      <c r="G61" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="H61" s="32">
+        <v>101665</v>
+      </c>
+      <c r="I61" s="32">
+        <v>123891</v>
+      </c>
+      <c r="J61" s="3">
+        <v>89.2</v>
+      </c>
+      <c r="K61" s="3">
+        <v>10.8</v>
+      </c>
+      <c r="L61" s="32">
+        <v>0</v>
+      </c>
+      <c r="M61" s="30">
+        <v>10</v>
+      </c>
+      <c r="N61" s="29"/>
+      <c r="O61" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="30">
+        <v>0</v>
+      </c>
+      <c r="B62" s="31">
+        <v>17462.3</v>
+      </c>
+      <c r="C62" s="30">
+        <v>14423</v>
+      </c>
+      <c r="D62" s="31">
+        <v>129803.13</v>
+      </c>
+      <c r="E62" s="30">
+        <v>0</v>
+      </c>
+      <c r="F62" s="32">
+        <v>161688</v>
+      </c>
+      <c r="G62" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="H62" s="32">
+        <v>99465</v>
+      </c>
+      <c r="I62" s="32">
+        <v>124199</v>
+      </c>
+      <c r="J62" s="3">
+        <v>89.2</v>
+      </c>
+      <c r="K62" s="3">
+        <v>10.8</v>
+      </c>
+      <c r="L62" s="32">
+        <v>0</v>
+      </c>
+      <c r="M62" s="30">
+        <v>10</v>
+      </c>
+      <c r="N62" s="29"/>
+      <c r="O62" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="30">
+        <v>0</v>
+      </c>
+      <c r="B63" s="31">
+        <v>142033.60999999999</v>
+      </c>
+      <c r="C63" s="30">
+        <v>117309</v>
+      </c>
+      <c r="D63" s="31">
+        <v>1055783.1499999999</v>
+      </c>
+      <c r="E63" s="30">
+        <v>0</v>
+      </c>
+      <c r="F63" s="32">
+        <v>1315126</v>
+      </c>
+      <c r="G63" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="H63" s="30">
+        <v>755015</v>
+      </c>
+      <c r="I63" s="31">
+        <v>1039448.2</v>
+      </c>
+      <c r="J63" s="3">
+        <v>89.2</v>
+      </c>
+      <c r="K63" s="3">
+        <v>10.8</v>
+      </c>
+      <c r="L63" s="32">
+        <v>0</v>
+      </c>
+      <c r="M63" s="30">
+        <v>1</v>
+      </c>
+      <c r="N63" s="29"/>
+      <c r="O63" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="30">
+        <v>0</v>
+      </c>
+      <c r="B64" s="31">
+        <v>59480.57</v>
+      </c>
+      <c r="C64" s="30">
+        <v>49127</v>
+      </c>
+      <c r="D64" s="31">
+        <v>442138.89</v>
+      </c>
+      <c r="E64" s="30">
+        <v>0</v>
+      </c>
+      <c r="F64" s="32">
+        <v>550746</v>
+      </c>
+      <c r="G64" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="H64" s="30">
+        <v>515138</v>
+      </c>
+      <c r="I64" s="31">
+        <v>819431.94</v>
+      </c>
+      <c r="J64" s="3">
+        <v>89.2</v>
+      </c>
+      <c r="K64" s="3">
+        <v>10.8</v>
+      </c>
+      <c r="L64" s="32">
+        <v>0</v>
+      </c>
+      <c r="M64" s="30">
+        <v>11</v>
+      </c>
+      <c r="N64" s="29"/>
+      <c r="O64" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -13687,15 +16749,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15888,12 +18950,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF1F056-CDA3-7A41-8A74-075468C8ABB2}">
   <dimension ref="A1:AY192"/>
   <sheetViews>
-    <sheetView topLeftCell="A172" zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -45405,8 +48467,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B191:C191">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="B3:B191">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -45417,8 +48479,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B191">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="B191:C191">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -45445,7 +48507,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -46746,156 +49808,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.5" style="5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3">
-        <v>23.5</v>
-      </c>
-      <c r="C2" s="3">
-        <v>76.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3">
-        <v>59.8</v>
-      </c>
-      <c r="C3" s="3">
-        <v>40.200000000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3">
-        <v>82.7</v>
-      </c>
-      <c r="C4" s="3">
-        <v>17.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3">
-        <v>91.4</v>
-      </c>
-      <c r="C5" s="3">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3">
-        <v>92.6</v>
-      </c>
-      <c r="C6" s="3">
-        <v>7.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3">
-        <v>92.9</v>
-      </c>
-      <c r="C7" s="3">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3">
-        <v>92.3</v>
-      </c>
-      <c r="C8" s="3">
-        <v>7.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="4">
-        <v>91</v>
-      </c>
-      <c r="C9" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="3">
-        <v>90.5</v>
-      </c>
-      <c r="C10" s="3">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="3">
-        <v>90.8</v>
-      </c>
-      <c r="C11" s="3">
-        <v>9.1999999999999993</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="3">
-        <v>89.2</v>
-      </c>
-      <c r="C12" s="3">
-        <v>10.8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>